<commit_message>
ajouts utilisateurs à mettre dans la bdd
</commit_message>
<xml_diff>
--- a/bdd/infos_bdd.xlsx
+++ b/bdd/infos_bdd.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marieeonnet/Documents/Documents - MacBook Pro de Marie/Cours_DUT_Caen/Projet2A/dut2021_pret_instruments_voyage/bdd/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1695B68-787C-B74E-AF99-355ACB9519E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DF53741-9EDC-0D43-A40F-400706567DBF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14520" yWindow="0" windowWidth="14280" windowHeight="18000" xr2:uid="{1C6F6E9A-B456-E643-B447-123029CC3B3E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{1C6F6E9A-B456-E643-B447-123029CC3B3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="218">
   <si>
     <t>Vil_num</t>
   </si>
@@ -267,9 +267,6 @@
     <t>RoninFire</t>
   </si>
   <si>
-    <t>NeverDream</t>
-  </si>
-  <si>
     <t>MusicMiss</t>
   </si>
   <si>
@@ -282,9 +279,6 @@
     <t>PoneyBlue</t>
   </si>
   <si>
-    <t>Mamalina</t>
-  </si>
-  <si>
     <t>RiverNaruto</t>
   </si>
   <si>
@@ -322,13 +316,385 @@
   </si>
   <si>
     <t>RockEmi</t>
+  </si>
+  <si>
+    <t>Pichard</t>
+  </si>
+  <si>
+    <t>Kilian</t>
+  </si>
+  <si>
+    <t>Massaly</t>
+  </si>
+  <si>
+    <t>Gaëlle</t>
+  </si>
+  <si>
+    <t>Romero</t>
+  </si>
+  <si>
+    <t>Mathias</t>
+  </si>
+  <si>
+    <t>Matator</t>
+  </si>
+  <si>
+    <t>Eonnet</t>
+  </si>
+  <si>
+    <t>Marie</t>
+  </si>
+  <si>
+    <t>Coupey</t>
+  </si>
+  <si>
+    <t>Noah</t>
+  </si>
+  <si>
+    <t>Queffelou</t>
+  </si>
+  <si>
+    <t>Mathieu</t>
+  </si>
+  <si>
+    <t>Snoopy</t>
+  </si>
+  <si>
+    <t>Desroches</t>
+  </si>
+  <si>
+    <t>Timothée</t>
+  </si>
+  <si>
+    <t>TimotheeDesroches@rhyta.com</t>
+  </si>
+  <si>
+    <t>Nahqua0ahsh</t>
+  </si>
+  <si>
+    <t>03.13.00.33.06</t>
+  </si>
+  <si>
+    <t>06.13.00.33.06</t>
+  </si>
+  <si>
+    <t>Karlotta</t>
+  </si>
+  <si>
+    <t>Monty</t>
+  </si>
+  <si>
+    <t>KarlottaMonty@jourrapide.com</t>
+  </si>
+  <si>
+    <t>Iewai4je8Loh</t>
+  </si>
+  <si>
+    <t>01.88.11.80.87</t>
+  </si>
+  <si>
+    <t>06.88.11.80.87</t>
+  </si>
+  <si>
+    <t>07.88.11.80.88</t>
+  </si>
+  <si>
+    <t>Iva</t>
+  </si>
+  <si>
+    <t>Routhier</t>
+  </si>
+  <si>
+    <t>IvaRouthier@armyspy.com</t>
+  </si>
+  <si>
+    <t>lah3MaiD</t>
+  </si>
+  <si>
+    <t>01.89.18.52.22</t>
+  </si>
+  <si>
+    <t>06.89.18.52.22</t>
+  </si>
+  <si>
+    <t>Julienne</t>
+  </si>
+  <si>
+    <t>Grandpré</t>
+  </si>
+  <si>
+    <t>JulienneGrandpre@jourrapide.com</t>
+  </si>
+  <si>
+    <t>johcieC3</t>
+  </si>
+  <si>
+    <t>06.95.20.40.91</t>
+  </si>
+  <si>
+    <t>02.95.20.40.91</t>
+  </si>
+  <si>
+    <t>Olivier</t>
+  </si>
+  <si>
+    <t>OlivierRouthier@dayrep.com</t>
+  </si>
+  <si>
+    <t>ieQuai7Ahk</t>
+  </si>
+  <si>
+    <t>04.61.94.78.79</t>
+  </si>
+  <si>
+    <t>07.61.94.78.79</t>
+  </si>
+  <si>
+    <t>Stéphane</t>
+  </si>
+  <si>
+    <t>Lanctot</t>
+  </si>
+  <si>
+    <t>StephaneLanctot@armyspy.com</t>
+  </si>
+  <si>
+    <t>Xe3aeXaiph</t>
+  </si>
+  <si>
+    <t>05.84.04.46.83</t>
+  </si>
+  <si>
+    <t>06.84.04.46.83</t>
+  </si>
+  <si>
+    <t>Octave</t>
+  </si>
+  <si>
+    <t>Bernier</t>
+  </si>
+  <si>
+    <t>OctaveBernier@rhyta.com</t>
+  </si>
+  <si>
+    <t>03.82.48.47.00</t>
+  </si>
+  <si>
+    <t>07.82.48.47.00</t>
+  </si>
+  <si>
+    <t>cam8Weeb</t>
+  </si>
+  <si>
+    <t>Olympia</t>
+  </si>
+  <si>
+    <t>Picard</t>
+  </si>
+  <si>
+    <t>OlympiaPicard@armyspy.com</t>
+  </si>
+  <si>
+    <t>Jai7Aitei</t>
+  </si>
+  <si>
+    <t>01.14.99.14.94</t>
+  </si>
+  <si>
+    <t>06.14.99.14.94</t>
+  </si>
+  <si>
+    <t>Mayhew</t>
+  </si>
+  <si>
+    <t>Dumont</t>
+  </si>
+  <si>
+    <t>MayhewDumont@jourrapide.com</t>
+  </si>
+  <si>
+    <t>chot2aiNai</t>
+  </si>
+  <si>
+    <t>02.39.95.74.69</t>
+  </si>
+  <si>
+    <t>07.39.95.74.69</t>
+  </si>
+  <si>
+    <t>Liane</t>
+  </si>
+  <si>
+    <t>Séguin</t>
+  </si>
+  <si>
+    <t>LianeSeguin@rhyta.com</t>
+  </si>
+  <si>
+    <t>quae0WaeW5oh</t>
+  </si>
+  <si>
+    <t>06.13.25.88.64</t>
+  </si>
+  <si>
+    <t>02.13.25.88.64</t>
+  </si>
+  <si>
+    <t>07.13.55.88.74</t>
+  </si>
+  <si>
+    <t>Claude</t>
+  </si>
+  <si>
+    <t>Michel</t>
+  </si>
+  <si>
+    <t>ClaudeMichel@rhyta.com</t>
+  </si>
+  <si>
+    <t>hohzohNg3</t>
+  </si>
+  <si>
+    <t>07.83.15.21.69</t>
+  </si>
+  <si>
+    <t>02.83.15.21.69</t>
+  </si>
+  <si>
+    <t>Edouard</t>
+  </si>
+  <si>
+    <t>Perillard</t>
+  </si>
+  <si>
+    <t>EdouardPerillard@dayrep.com</t>
+  </si>
+  <si>
+    <t>Quaig8ar9</t>
+  </si>
+  <si>
+    <t>06.27.24.64.52</t>
+  </si>
+  <si>
+    <t>03.27.24.64.52</t>
+  </si>
+  <si>
+    <t>Carole</t>
+  </si>
+  <si>
+    <t>Pichette</t>
+  </si>
+  <si>
+    <t>CarolePichette@rhyta.com</t>
+  </si>
+  <si>
+    <t>Iegh3vagai</t>
+  </si>
+  <si>
+    <t>04.52.64.99.08</t>
+  </si>
+  <si>
+    <t>07.52.64.99.08</t>
+  </si>
+  <si>
+    <t>31/11/2001</t>
+  </si>
+  <si>
+    <t>Roger</t>
+  </si>
+  <si>
+    <t>Brunault</t>
+  </si>
+  <si>
+    <t>RogerBrunault@rhyta.com</t>
+  </si>
+  <si>
+    <t>Goohaim3</t>
+  </si>
+  <si>
+    <t>07.29.13.89.67</t>
+  </si>
+  <si>
+    <t>02.29.13.89.67</t>
+  </si>
+  <si>
+    <t>PichardKilian@armyspy.com</t>
+  </si>
+  <si>
+    <t>RomeroMathias@rhyta.com</t>
+  </si>
+  <si>
+    <t>MassalyGaelle@jourrapide.com</t>
+  </si>
+  <si>
+    <t>EonnetMarie@dayrep.com</t>
+  </si>
+  <si>
+    <t>CoupeyNoah@dayrep.com</t>
+  </si>
+  <si>
+    <t>QueffelouMathieu@armyspy.com</t>
+  </si>
+  <si>
+    <t>Vahwo6cai</t>
+  </si>
+  <si>
+    <t>06.01.58.17.82</t>
+  </si>
+  <si>
+    <t>02.01.58.17.82</t>
+  </si>
+  <si>
+    <t>naez4Aizei</t>
+  </si>
+  <si>
+    <t>07.95.50.98.35</t>
+  </si>
+  <si>
+    <t>02.95.50.98.35</t>
+  </si>
+  <si>
+    <t>Seiphae1ohM</t>
+  </si>
+  <si>
+    <t>05.42.20.53.03</t>
+  </si>
+  <si>
+    <t>06.42.20.53.03</t>
+  </si>
+  <si>
+    <t>aicou1iePh</t>
+  </si>
+  <si>
+    <t>07.30.20.16.36</t>
+  </si>
+  <si>
+    <t>02.30.20.16.36</t>
+  </si>
+  <si>
+    <t>ooqu1Mahxoh</t>
+  </si>
+  <si>
+    <t>06.24.81.80.46</t>
+  </si>
+  <si>
+    <t>02.24.81.80.46</t>
+  </si>
+  <si>
+    <t>yoF9joh7xee</t>
+  </si>
+  <si>
+    <t>01.92.08.94.99</t>
+  </si>
+  <si>
+    <t>07.92.08.94.99</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -352,6 +718,41 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -361,7 +762,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -384,22 +785,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -417,19 +808,35 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -744,8 +1151,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D70755CD-10D4-DA48-863B-E92693C8657B}">
   <dimension ref="B2:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -756,9 +1163,9 @@
     <col min="6" max="6" width="22.33203125" customWidth="1"/>
     <col min="7" max="7" width="20.83203125" customWidth="1"/>
     <col min="8" max="8" width="26.6640625" customWidth="1"/>
-    <col min="9" max="9" width="17" customWidth="1"/>
+    <col min="9" max="9" width="37.6640625" customWidth="1"/>
     <col min="10" max="10" width="15.83203125" customWidth="1"/>
-    <col min="11" max="11" width="16.33203125" customWidth="1"/>
+    <col min="11" max="11" width="22.6640625" customWidth="1"/>
     <col min="12" max="12" width="17.6640625" customWidth="1"/>
     <col min="13" max="13" width="19.5" customWidth="1"/>
   </cols>
@@ -1178,429 +1585,767 @@
       <c r="M26" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="N26" s="7"/>
+      <c r="N26" s="6"/>
     </row>
     <row r="27" spans="2:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="B27" s="6">
+      <c r="B27" s="8">
         <v>1</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C27" s="8">
         <v>5</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="7"/>
-      <c r="M27" s="7"/>
-      <c r="N27" s="7"/>
-    </row>
-    <row r="28" spans="2:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="B28" s="6">
+      <c r="E27" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="G27" s="9">
+        <v>37231</v>
+      </c>
+      <c r="H27" s="9">
+        <v>44178</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="J27" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="K27" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="L27" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
+    </row>
+    <row r="28" spans="2:14" ht="19" x14ac:dyDescent="0.2">
+      <c r="B28" s="8">
         <v>2</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C28" s="8">
         <v>1</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D28" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="H28" s="9">
+        <v>44146</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="J28" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="K28" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="L28" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="M28" s="8"/>
+      <c r="N28" s="8"/>
+    </row>
+    <row r="29" spans="2:14" ht="19" x14ac:dyDescent="0.2">
+      <c r="B29" s="8">
+        <v>3</v>
+      </c>
+      <c r="C29" s="8">
+        <v>4</v>
+      </c>
+      <c r="D29" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="7"/>
-      <c r="K28" s="7"/>
-      <c r="L28" s="7"/>
-      <c r="M28" s="7"/>
-      <c r="N28" s="7"/>
-    </row>
-    <row r="29" spans="2:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="B29" s="6">
+      <c r="E29" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="G29" s="9">
+        <v>37243</v>
+      </c>
+      <c r="H29" s="9">
+        <v>43844</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="J29" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="K29" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="L29" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="M29" s="8"/>
+      <c r="N29" s="8"/>
+    </row>
+    <row r="30" spans="2:14" ht="19" x14ac:dyDescent="0.2">
+      <c r="B30" s="8">
+        <v>4</v>
+      </c>
+      <c r="C30" s="8">
+        <v>10</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="G30" s="9">
+        <v>36588</v>
+      </c>
+      <c r="H30" s="9">
+        <v>43893</v>
+      </c>
+      <c r="I30" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="J30" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="K30" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="L30" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="M30" s="8"/>
+      <c r="N30" s="8"/>
+    </row>
+    <row r="31" spans="2:14" ht="19" x14ac:dyDescent="0.2">
+      <c r="B31" s="8">
+        <v>5</v>
+      </c>
+      <c r="C31" s="8">
+        <v>20</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="G31" s="9">
+        <v>37046</v>
+      </c>
+      <c r="H31" s="9">
+        <v>43996</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="J31" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="K31" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="L31" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="M31" s="8"/>
+      <c r="N31" s="8"/>
+    </row>
+    <row r="32" spans="2:14" ht="19" x14ac:dyDescent="0.2">
+      <c r="B32" s="8">
+        <v>6</v>
+      </c>
+      <c r="C32" s="8">
+        <v>6</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="G32" s="9">
+        <v>36970</v>
+      </c>
+      <c r="H32" s="9">
+        <v>44124</v>
+      </c>
+      <c r="I32" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="J32" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="K32" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="L32" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="M32" s="8"/>
+      <c r="N32" s="8"/>
+    </row>
+    <row r="33" spans="2:14" ht="19" x14ac:dyDescent="0.2">
+      <c r="B33" s="8">
+        <v>7</v>
+      </c>
+      <c r="C33" s="8">
+        <v>9</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="G33" s="9">
+        <v>36773</v>
+      </c>
+      <c r="H33" s="9">
+        <v>44042</v>
+      </c>
+      <c r="I33" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="J33" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="K33" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="L33" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="M33" s="8"/>
+      <c r="N33" s="8"/>
+    </row>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B34" s="8">
+        <v>8</v>
+      </c>
+      <c r="C34" s="8">
+        <v>11</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="G34" s="9">
+        <v>34095</v>
+      </c>
+      <c r="H34" s="9">
+        <v>40533</v>
+      </c>
+      <c r="I34" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="J34" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="K34" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="L34" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="M34" s="8"/>
+      <c r="N34" s="8"/>
+    </row>
+    <row r="35" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B35" s="8">
+        <v>9</v>
+      </c>
+      <c r="C35" s="8">
+        <v>14</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="G35" s="9">
+        <v>27565</v>
+      </c>
+      <c r="H35" s="9">
+        <v>40240</v>
+      </c>
+      <c r="I35" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="J35" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="K35" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="L35" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="M35" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="N35" s="8"/>
+    </row>
+    <row r="36" spans="2:14" ht="19" x14ac:dyDescent="0.2">
+      <c r="B36" s="8">
+        <v>10</v>
+      </c>
+      <c r="C36" s="8">
+        <v>15</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="G36" s="9">
+        <v>26789</v>
+      </c>
+      <c r="H36" s="9">
+        <v>40933</v>
+      </c>
+      <c r="I36" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="J36" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="K36" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="L36" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="M36" s="8"/>
+      <c r="N36" s="8"/>
+    </row>
+    <row r="37" spans="2:14" ht="19" x14ac:dyDescent="0.2">
+      <c r="B37" s="8">
+        <v>11</v>
+      </c>
+      <c r="C37" s="8">
+        <v>19</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="G37" s="9">
+        <v>29468</v>
+      </c>
+      <c r="H37" s="9">
+        <v>39913</v>
+      </c>
+      <c r="I37" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="J37" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="K37" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="L37" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="M37" s="8"/>
+      <c r="N37" s="8"/>
+    </row>
+    <row r="38" spans="2:14" ht="19" x14ac:dyDescent="0.2">
+      <c r="B38" s="8">
+        <v>12</v>
+      </c>
+      <c r="C38" s="8">
+        <v>2</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="G38" s="9">
+        <v>28337</v>
+      </c>
+      <c r="H38" s="9">
+        <v>40179</v>
+      </c>
+      <c r="I38" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="J38" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="K38" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="L38" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="M38" s="8"/>
+      <c r="N38" s="8"/>
+    </row>
+    <row r="39" spans="2:14" ht="19" x14ac:dyDescent="0.2">
+      <c r="B39" s="8">
+        <v>13</v>
+      </c>
+      <c r="C39" s="8">
         <v>3</v>
       </c>
-      <c r="C29" s="6">
-        <v>4</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="7"/>
-      <c r="L29" s="7"/>
-      <c r="M29" s="7"/>
-      <c r="N29" s="7"/>
-    </row>
-    <row r="30" spans="2:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="B30" s="6">
-        <v>4</v>
-      </c>
-      <c r="C30" s="6">
-        <v>10</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="7"/>
-      <c r="K30" s="7"/>
-      <c r="L30" s="7"/>
-      <c r="M30" s="7"/>
-      <c r="N30" s="7"/>
-    </row>
-    <row r="31" spans="2:14" ht="17" x14ac:dyDescent="0.2">
-      <c r="B31" s="6">
-        <v>5</v>
-      </c>
-      <c r="C31" s="6">
+      <c r="D39" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="G39" s="9">
+        <v>27435</v>
+      </c>
+      <c r="H39" s="9">
+        <v>41917</v>
+      </c>
+      <c r="I39" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="J39" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="K39" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="L39" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="M39" s="8"/>
+      <c r="N39" s="8"/>
+    </row>
+    <row r="40" spans="2:14" ht="19" x14ac:dyDescent="0.2">
+      <c r="B40" s="8">
+        <v>14</v>
+      </c>
+      <c r="C40" s="8">
+        <v>7</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="G40" s="9">
+        <v>31859</v>
+      </c>
+      <c r="H40" s="9">
+        <v>40362</v>
+      </c>
+      <c r="I40" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="J40" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="K40" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="L40" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="M40" s="8"/>
+      <c r="N40" s="8"/>
+    </row>
+    <row r="41" spans="2:14" ht="19" x14ac:dyDescent="0.2">
+      <c r="B41" s="8">
+        <v>15</v>
+      </c>
+      <c r="C41" s="8">
+        <v>8</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="G41" s="14">
+        <v>28506</v>
+      </c>
+      <c r="H41" s="14">
+        <v>42368</v>
+      </c>
+      <c r="I41" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="J41" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="K41" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="L41" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="M41" s="8"/>
+      <c r="N41" s="8"/>
+    </row>
+    <row r="42" spans="2:14" ht="19" x14ac:dyDescent="0.2">
+      <c r="B42" s="8">
+        <v>16</v>
+      </c>
+      <c r="C42" s="8">
+        <v>13</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="G42" s="9">
+        <v>26846</v>
+      </c>
+      <c r="H42" s="9">
+        <v>44177</v>
+      </c>
+      <c r="I42" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="J42" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="K42" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="L42" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="M42" s="8"/>
+      <c r="N42" s="8"/>
+    </row>
+    <row r="43" spans="2:14" ht="19" x14ac:dyDescent="0.2">
+      <c r="B43" s="11">
+        <v>17</v>
+      </c>
+      <c r="C43" s="8">
+        <v>12</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="G43" s="9">
+        <v>33439</v>
+      </c>
+      <c r="H43" s="9">
+        <v>43047</v>
+      </c>
+      <c r="I43" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="J43" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="K43" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="L43" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="M43" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="N43" s="8"/>
+    </row>
+    <row r="44" spans="2:14" ht="19" x14ac:dyDescent="0.2">
+      <c r="B44" s="11">
+        <v>18</v>
+      </c>
+      <c r="C44" s="8">
+        <v>16</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="F44" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="G44" s="9">
+        <v>28991</v>
+      </c>
+      <c r="H44" s="9">
+        <v>41517</v>
+      </c>
+      <c r="I44" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="J44" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="K44" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="L44" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="M44" s="8"/>
+      <c r="N44" s="8"/>
+    </row>
+    <row r="45" spans="2:14" ht="19" x14ac:dyDescent="0.2">
+      <c r="B45" s="11">
+        <v>19</v>
+      </c>
+      <c r="C45" s="8">
+        <v>18</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="G45" s="9">
+        <v>34480</v>
+      </c>
+      <c r="H45" s="9">
+        <v>43748</v>
+      </c>
+      <c r="I45" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="J45" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="K45" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="L45" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="M45" s="8"/>
+      <c r="N45" s="8"/>
+    </row>
+    <row r="46" spans="2:14" ht="19" x14ac:dyDescent="0.2">
+      <c r="B46" s="11">
         <v>20</v>
       </c>
-      <c r="D31" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
-      <c r="K31" s="7"/>
-      <c r="L31" s="7"/>
-      <c r="M31" s="7"/>
-      <c r="N31" s="7"/>
-    </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B32" s="7">
-        <v>6</v>
-      </c>
-      <c r="C32" s="7">
-        <v>6</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
-      <c r="J32" s="7"/>
-      <c r="K32" s="7"/>
-      <c r="L32" s="7"/>
-      <c r="M32" s="7"/>
-      <c r="N32" s="7"/>
-    </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B33" s="7">
-        <v>7</v>
-      </c>
-      <c r="C33" s="7">
-        <v>9</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="7"/>
-      <c r="K33" s="7"/>
-      <c r="L33" s="7"/>
-      <c r="M33" s="7"/>
-      <c r="N33" s="7"/>
-    </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B34" s="7">
-        <v>8</v>
-      </c>
-      <c r="C34" s="7">
-        <v>11</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
-      <c r="I34" s="7"/>
-      <c r="J34" s="7"/>
-      <c r="K34" s="7"/>
-      <c r="L34" s="7"/>
-      <c r="M34" s="7"/>
-      <c r="N34" s="7"/>
-    </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B35" s="7">
-        <v>9</v>
-      </c>
-      <c r="C35" s="7">
-        <v>14</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="7"/>
-      <c r="I35" s="7"/>
-      <c r="J35" s="7"/>
-      <c r="K35" s="7"/>
-      <c r="L35" s="7"/>
-      <c r="M35" s="7"/>
-      <c r="N35" s="7"/>
-    </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B36" s="7">
-        <v>10</v>
-      </c>
-      <c r="C36" s="7">
-        <v>15</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="7"/>
-      <c r="I36" s="7"/>
-      <c r="J36" s="7"/>
-      <c r="K36" s="7"/>
-      <c r="L36" s="7"/>
-      <c r="M36" s="7"/>
-      <c r="N36" s="7"/>
-    </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B37" s="7">
-        <v>11</v>
-      </c>
-      <c r="C37" s="7">
-        <v>19</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="7"/>
-      <c r="I37" s="7"/>
-      <c r="J37" s="7"/>
-      <c r="K37" s="7"/>
-      <c r="L37" s="7"/>
-      <c r="M37" s="7"/>
-      <c r="N37" s="7"/>
-    </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B38" s="7">
-        <v>12</v>
-      </c>
-      <c r="C38" s="7">
-        <v>2</v>
-      </c>
-      <c r="D38" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
-      <c r="I38" s="7"/>
-      <c r="J38" s="7"/>
-      <c r="K38" s="7"/>
-      <c r="L38" s="7"/>
-      <c r="M38" s="7"/>
-      <c r="N38" s="7"/>
-    </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B39" s="7">
-        <v>13</v>
-      </c>
-      <c r="C39" s="7">
-        <v>3</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="7"/>
-      <c r="I39" s="7"/>
-      <c r="J39" s="7"/>
-      <c r="K39" s="7"/>
-      <c r="L39" s="7"/>
-      <c r="M39" s="7"/>
-      <c r="N39" s="7"/>
-    </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B40" s="7">
-        <v>14</v>
-      </c>
-      <c r="C40" s="7">
-        <v>7</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="7"/>
-      <c r="I40" s="7"/>
-      <c r="J40" s="7"/>
-      <c r="K40" s="7"/>
-      <c r="L40" s="7"/>
-      <c r="M40" s="7"/>
-      <c r="N40" s="7"/>
-    </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B41" s="7">
-        <v>15</v>
-      </c>
-      <c r="C41" s="7">
-        <v>8</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="7"/>
-      <c r="I41" s="7"/>
-      <c r="J41" s="7"/>
-      <c r="K41" s="7"/>
-      <c r="L41" s="7"/>
-      <c r="M41" s="7"/>
-      <c r="N41" s="7"/>
-    </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B42" s="7">
-        <v>16</v>
-      </c>
-      <c r="C42" s="7">
-        <v>13</v>
-      </c>
-      <c r="D42" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="7"/>
-      <c r="I42" s="7"/>
-      <c r="J42" s="7"/>
-      <c r="K42" s="7"/>
-      <c r="L42" s="7"/>
-      <c r="M42" s="7"/>
-      <c r="N42" s="7"/>
-    </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B43" s="8">
+      <c r="C46" s="8">
         <v>17</v>
       </c>
-      <c r="C43" s="7">
-        <v>12</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="7"/>
-      <c r="I43" s="7"/>
-      <c r="J43" s="7"/>
-      <c r="K43" s="7"/>
-      <c r="L43" s="7"/>
-      <c r="M43" s="7"/>
-      <c r="N43" s="7"/>
-    </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B44" s="8">
-        <v>18</v>
-      </c>
-      <c r="C44" s="7">
-        <v>16</v>
-      </c>
-      <c r="D44" s="7" t="s">
+      <c r="D46" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7"/>
-      <c r="G44" s="7"/>
-      <c r="H44" s="7"/>
-      <c r="I44" s="7"/>
-      <c r="J44" s="7"/>
-      <c r="K44" s="7"/>
-      <c r="L44" s="7"/>
-      <c r="M44" s="7"/>
-      <c r="N44" s="7"/>
-    </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B45" s="8">
-        <v>19</v>
-      </c>
-      <c r="C45" s="7">
-        <v>18</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7"/>
-      <c r="G45" s="7"/>
-      <c r="H45" s="7"/>
-      <c r="I45" s="7"/>
-      <c r="J45" s="7"/>
-      <c r="K45" s="7"/>
-      <c r="L45" s="7"/>
-      <c r="M45" s="7"/>
-      <c r="N45" s="7"/>
-    </row>
-    <row r="46" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B46" s="8">
-        <v>20</v>
-      </c>
-      <c r="C46" s="7">
-        <v>17</v>
-      </c>
-      <c r="D46" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="E46" s="7"/>
-      <c r="F46" s="7"/>
-      <c r="G46" s="7"/>
-      <c r="H46" s="7"/>
-      <c r="I46" s="7"/>
-      <c r="J46" s="7"/>
-      <c r="K46" s="7"/>
-      <c r="L46" s="7"/>
-      <c r="M46" s="7"/>
-      <c r="N46" s="7"/>
+      <c r="E46" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="G46" s="9">
+        <v>36294</v>
+      </c>
+      <c r="H46" s="9">
+        <v>43966</v>
+      </c>
+      <c r="I46" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="J46" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="K46" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="L46" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="M46" s="8"/>
+      <c r="N46" s="8"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I34" r:id="rId1" xr:uid="{BA1FB798-E09E-724C-B38A-559701AF93EA}"/>
+    <hyperlink ref="I35" r:id="rId2" xr:uid="{0A154888-FD69-F744-9B89-4A33C50548E0}"/>
+    <hyperlink ref="I40" r:id="rId3" xr:uid="{46CE5D2A-88C6-DA46-903D-F5C3A733F1D6}"/>
+    <hyperlink ref="I42" r:id="rId4" xr:uid="{60D2DBEA-D762-BE45-8600-702D055198DC}"/>
+    <hyperlink ref="I43" r:id="rId5" xr:uid="{DEB3DF1B-B6CC-0D43-A09D-E53BBA4B3CB0}"/>
+    <hyperlink ref="I44" r:id="rId6" xr:uid="{BF0748C4-7B27-5E45-9364-E5B380285102}"/>
+    <hyperlink ref="I27" r:id="rId7" xr:uid="{2AC29F59-C222-534B-AC13-140A15EECCC9}"/>
+    <hyperlink ref="I28" r:id="rId8" xr:uid="{D250BC60-783E-4640-A68B-A9B48D7EC083}"/>
+    <hyperlink ref="I29" r:id="rId9" xr:uid="{0C914855-49FF-4E4F-B5E7-2448291ECFBB}"/>
+    <hyperlink ref="I30" r:id="rId10" xr:uid="{A0902495-50C9-EF4F-895F-AB91E8CEB59F}"/>
+    <hyperlink ref="I31" r:id="rId11" xr:uid="{91B0895A-5126-1C4C-8332-B548BB377A77}"/>
+    <hyperlink ref="I32" r:id="rId12" xr:uid="{EBC71EFF-54C7-3E4A-9B89-A57AAD183F48}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ajout de la base de donnée en mySql
</commit_message>
<xml_diff>
--- a/bdd/infos_bdd.xlsx
+++ b/bdd/infos_bdd.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marieeonnet/Documents/Documents - MacBook Pro de Marie/Cours_DUT_Caen/Projet2A/dut2021_pret_instruments_voyage/bdd/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DF53741-9EDC-0D43-A40F-400706567DBF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A06250C9-7DB9-444C-9E20-6E5CA9779B71}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{1C6F6E9A-B456-E643-B447-123029CC3B3E}"/>
+    <workbookView xWindow="17020" yWindow="0" windowWidth="11780" windowHeight="18000" xr2:uid="{1C6F6E9A-B456-E643-B447-123029CC3B3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -264,9 +264,6 @@
     <t>uti_portable_2</t>
   </si>
   <si>
-    <t>RoninFire</t>
-  </si>
-  <si>
     <t>MusicMiss</t>
   </si>
   <si>
@@ -688,6 +685,9 @@
   </si>
   <si>
     <t>07.92.08.94.99</t>
+  </si>
+  <si>
+    <t>clarinetDuet</t>
   </si>
 </sst>
 </file>
@@ -1151,8 +1151,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D70755CD-10D4-DA48-863B-E92693C8657B}">
   <dimension ref="B2:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="I24" workbookViewId="0">
+      <selection activeCell="L46" sqref="L46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1595,13 +1595,13 @@
         <v>5</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>76</v>
+        <v>217</v>
       </c>
       <c r="E27" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F27" s="8" t="s">
         <v>94</v>
-      </c>
-      <c r="F27" s="8" t="s">
-        <v>95</v>
       </c>
       <c r="G27" s="9">
         <v>37231</v>
@@ -1610,16 +1610,16 @@
         <v>44178</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J27" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="K27" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="L27" s="8" t="s">
         <v>215</v>
-      </c>
-      <c r="K27" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="L27" s="8" t="s">
-        <v>216</v>
       </c>
       <c r="M27" s="8"/>
       <c r="N27" s="8"/>
@@ -1632,31 +1632,31 @@
         <v>1</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E28" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="F28" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="F28" s="8" t="s">
-        <v>99</v>
-      </c>
       <c r="G28" s="8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H28" s="9">
         <v>44146</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J28" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="K28" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="K28" s="8" t="s">
+      <c r="L28" s="13" t="s">
         <v>213</v>
-      </c>
-      <c r="L28" s="13" t="s">
-        <v>214</v>
       </c>
       <c r="M28" s="8"/>
       <c r="N28" s="8"/>
@@ -1669,13 +1669,13 @@
         <v>4</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E29" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="F29" s="8" t="s">
         <v>96</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>97</v>
       </c>
       <c r="G29" s="9">
         <v>37243</v>
@@ -1684,16 +1684,16 @@
         <v>43844</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J29" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="K29" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="K29" s="8" t="s">
+      <c r="L29" s="13" t="s">
         <v>210</v>
-      </c>
-      <c r="L29" s="13" t="s">
-        <v>211</v>
       </c>
       <c r="M29" s="8"/>
       <c r="N29" s="8"/>
@@ -1706,13 +1706,13 @@
         <v>10</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E30" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="F30" s="8" t="s">
         <v>101</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>102</v>
       </c>
       <c r="G30" s="9">
         <v>36588</v>
@@ -1721,16 +1721,16 @@
         <v>43893</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J30" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="K30" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="L30" s="13" t="s">
         <v>206</v>
-      </c>
-      <c r="K30" s="13" t="s">
-        <v>208</v>
-      </c>
-      <c r="L30" s="13" t="s">
-        <v>207</v>
       </c>
       <c r="M30" s="8"/>
       <c r="N30" s="8"/>
@@ -1743,13 +1743,13 @@
         <v>20</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E31" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="F31" s="8" t="s">
         <v>103</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>104</v>
       </c>
       <c r="G31" s="9">
         <v>37046</v>
@@ -1758,16 +1758,16 @@
         <v>43996</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J31" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="K31" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="K31" s="13" t="s">
+      <c r="L31" s="13" t="s">
         <v>204</v>
-      </c>
-      <c r="L31" s="13" t="s">
-        <v>205</v>
       </c>
       <c r="M31" s="8"/>
       <c r="N31" s="8"/>
@@ -1780,13 +1780,13 @@
         <v>6</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E32" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="F32" s="8" t="s">
         <v>105</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>106</v>
       </c>
       <c r="G32" s="9">
         <v>36970</v>
@@ -1795,16 +1795,16 @@
         <v>44124</v>
       </c>
       <c r="I32" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="J32" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="J32" s="8" t="s">
+      <c r="K32" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="K32" s="8" t="s">
+      <c r="L32" s="13" t="s">
         <v>201</v>
-      </c>
-      <c r="L32" s="13" t="s">
-        <v>202</v>
       </c>
       <c r="M32" s="8"/>
       <c r="N32" s="8"/>
@@ -1817,13 +1817,13 @@
         <v>9</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E33" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="F33" s="8" t="s">
         <v>188</v>
-      </c>
-      <c r="F33" s="8" t="s">
-        <v>189</v>
       </c>
       <c r="G33" s="9">
         <v>36773</v>
@@ -1832,16 +1832,16 @@
         <v>44042</v>
       </c>
       <c r="I33" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="J33" s="13" t="s">
         <v>190</v>
       </c>
-      <c r="J33" s="13" t="s">
+      <c r="K33" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="K33" s="8" t="s">
+      <c r="L33" s="13" t="s">
         <v>192</v>
-      </c>
-      <c r="L33" s="13" t="s">
-        <v>193</v>
       </c>
       <c r="M33" s="8"/>
       <c r="N33" s="8"/>
@@ -1854,13 +1854,13 @@
         <v>11</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E34" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="F34" s="8" t="s">
         <v>108</v>
-      </c>
-      <c r="F34" s="8" t="s">
-        <v>109</v>
       </c>
       <c r="G34" s="9">
         <v>34095</v>
@@ -1869,16 +1869,16 @@
         <v>40533</v>
       </c>
       <c r="I34" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="J34" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="J34" s="12" t="s">
+      <c r="K34" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="L34" s="8" t="s">
         <v>111</v>
-      </c>
-      <c r="K34" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="L34" s="8" t="s">
-        <v>112</v>
       </c>
       <c r="M34" s="8"/>
       <c r="N34" s="8"/>
@@ -1891,13 +1891,13 @@
         <v>14</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E35" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="F35" s="8" t="s">
         <v>114</v>
-      </c>
-      <c r="F35" s="8" t="s">
-        <v>115</v>
       </c>
       <c r="G35" s="9">
         <v>27565</v>
@@ -1906,19 +1906,19 @@
         <v>40240</v>
       </c>
       <c r="I35" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="J35" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="J35" s="8" t="s">
+      <c r="K35" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="L35" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="K35" s="12" t="s">
+      <c r="M35" s="12" t="s">
         <v>119</v>
-      </c>
-      <c r="L35" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="M35" s="12" t="s">
-        <v>120</v>
       </c>
       <c r="N35" s="8"/>
     </row>
@@ -1930,13 +1930,13 @@
         <v>15</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E36" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="F36" s="8" t="s">
         <v>121</v>
-      </c>
-      <c r="F36" s="8" t="s">
-        <v>122</v>
       </c>
       <c r="G36" s="9">
         <v>26789</v>
@@ -1945,16 +1945,16 @@
         <v>40933</v>
       </c>
       <c r="I36" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="J36" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="J36" s="8" t="s">
+      <c r="K36" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="L36" s="13" t="s">
         <v>124</v>
-      </c>
-      <c r="K36" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="L36" s="13" t="s">
-        <v>125</v>
       </c>
       <c r="M36" s="8"/>
       <c r="N36" s="8"/>
@@ -1967,13 +1967,13 @@
         <v>19</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E37" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="F37" s="8" t="s">
         <v>127</v>
-      </c>
-      <c r="F37" s="8" t="s">
-        <v>128</v>
       </c>
       <c r="G37" s="9">
         <v>29468</v>
@@ -1982,16 +1982,16 @@
         <v>39913</v>
       </c>
       <c r="I37" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="J37" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="J37" s="13" t="s">
+      <c r="K37" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="K37" s="13" t="s">
+      <c r="L37" s="13" t="s">
         <v>131</v>
-      </c>
-      <c r="L37" s="13" t="s">
-        <v>132</v>
       </c>
       <c r="M37" s="8"/>
       <c r="N37" s="8"/>
@@ -2004,13 +2004,13 @@
         <v>2</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G38" s="9">
         <v>28337</v>
@@ -2019,16 +2019,16 @@
         <v>40179</v>
       </c>
       <c r="I38" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="J38" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="J38" s="13" t="s">
+      <c r="K38" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="L38" s="13" t="s">
         <v>135</v>
-      </c>
-      <c r="K38" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="L38" s="13" t="s">
-        <v>136</v>
       </c>
       <c r="M38" s="8"/>
       <c r="N38" s="8"/>
@@ -2041,13 +2041,13 @@
         <v>3</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E39" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="F39" s="8" t="s">
         <v>138</v>
-      </c>
-      <c r="F39" s="8" t="s">
-        <v>139</v>
       </c>
       <c r="G39" s="9">
         <v>27435</v>
@@ -2056,16 +2056,16 @@
         <v>41917</v>
       </c>
       <c r="I39" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="J39" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="J39" s="13" t="s">
+      <c r="K39" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="L39" s="13" t="s">
         <v>141</v>
-      </c>
-      <c r="K39" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="L39" s="13" t="s">
-        <v>142</v>
       </c>
       <c r="M39" s="8"/>
       <c r="N39" s="8"/>
@@ -2078,13 +2078,13 @@
         <v>7</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E40" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="F40" s="8" t="s">
         <v>144</v>
-      </c>
-      <c r="F40" s="8" t="s">
-        <v>145</v>
       </c>
       <c r="G40" s="9">
         <v>31859</v>
@@ -2093,16 +2093,16 @@
         <v>40362</v>
       </c>
       <c r="I40" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="J40" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="K40" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="L40" s="13" t="s">
         <v>146</v>
-      </c>
-      <c r="J40" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="K40" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="L40" s="13" t="s">
-        <v>147</v>
       </c>
       <c r="M40" s="8"/>
       <c r="N40" s="8"/>
@@ -2115,13 +2115,13 @@
         <v>8</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E41" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="F41" s="8" t="s">
         <v>150</v>
-      </c>
-      <c r="F41" s="8" t="s">
-        <v>151</v>
       </c>
       <c r="G41" s="14">
         <v>28506</v>
@@ -2130,16 +2130,16 @@
         <v>42368</v>
       </c>
       <c r="I41" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="J41" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="J41" s="13" t="s">
+      <c r="K41" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="L41" s="13" t="s">
         <v>153</v>
-      </c>
-      <c r="K41" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="L41" s="13" t="s">
-        <v>154</v>
       </c>
       <c r="M41" s="8"/>
       <c r="N41" s="8"/>
@@ -2152,13 +2152,13 @@
         <v>13</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E42" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="F42" s="8" t="s">
         <v>156</v>
-      </c>
-      <c r="F42" s="8" t="s">
-        <v>157</v>
       </c>
       <c r="G42" s="9">
         <v>26846</v>
@@ -2167,16 +2167,16 @@
         <v>44177</v>
       </c>
       <c r="I42" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="J42" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="J42" s="13" t="s">
+      <c r="K42" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="L42" s="13" t="s">
         <v>159</v>
-      </c>
-      <c r="K42" s="13" t="s">
-        <v>161</v>
-      </c>
-      <c r="L42" s="13" t="s">
-        <v>160</v>
       </c>
       <c r="M42" s="8"/>
       <c r="N42" s="8"/>
@@ -2189,13 +2189,13 @@
         <v>12</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E43" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="F43" s="8" t="s">
         <v>162</v>
-      </c>
-      <c r="F43" s="8" t="s">
-        <v>163</v>
       </c>
       <c r="G43" s="9">
         <v>33439</v>
@@ -2204,19 +2204,19 @@
         <v>43047</v>
       </c>
       <c r="I43" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="J43" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="J43" s="8" t="s">
+      <c r="K43" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="K43" s="8" t="s">
+      <c r="L43" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="L43" s="13" t="s">
+      <c r="M43" s="13" t="s">
         <v>167</v>
-      </c>
-      <c r="M43" s="13" t="s">
-        <v>168</v>
       </c>
       <c r="N43" s="8"/>
     </row>
@@ -2228,13 +2228,13 @@
         <v>16</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E44" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="F44" s="11" t="s">
         <v>169</v>
-      </c>
-      <c r="F44" s="11" t="s">
-        <v>170</v>
       </c>
       <c r="G44" s="9">
         <v>28991</v>
@@ -2243,16 +2243,16 @@
         <v>41517</v>
       </c>
       <c r="I44" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="J44" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="J44" s="8" t="s">
+      <c r="K44" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="K44" s="8" t="s">
+      <c r="L44" s="13" t="s">
         <v>173</v>
-      </c>
-      <c r="L44" s="13" t="s">
-        <v>174</v>
       </c>
       <c r="M44" s="8"/>
       <c r="N44" s="8"/>
@@ -2265,13 +2265,13 @@
         <v>18</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E45" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="F45" s="8" t="s">
         <v>175</v>
-      </c>
-      <c r="F45" s="8" t="s">
-        <v>176</v>
       </c>
       <c r="G45" s="9">
         <v>34480</v>
@@ -2280,16 +2280,16 @@
         <v>43748</v>
       </c>
       <c r="I45" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="J45" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="J45" s="13" t="s">
+      <c r="K45" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="K45" s="8" t="s">
+      <c r="L45" s="13" t="s">
         <v>179</v>
-      </c>
-      <c r="L45" s="13" t="s">
-        <v>180</v>
       </c>
       <c r="M45" s="8"/>
       <c r="N45" s="8"/>
@@ -2302,13 +2302,13 @@
         <v>17</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E46" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="F46" s="8" t="s">
         <v>181</v>
-      </c>
-      <c r="F46" s="8" t="s">
-        <v>182</v>
       </c>
       <c r="G46" s="9">
         <v>36294</v>
@@ -2317,16 +2317,16 @@
         <v>43966</v>
       </c>
       <c r="I46" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="J46" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="J46" s="8" t="s">
+      <c r="K46" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="L46" s="13" t="s">
         <v>184</v>
-      </c>
-      <c r="K46" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="L46" s="13" t="s">
-        <v>185</v>
       </c>
       <c r="M46" s="8"/>
       <c r="N46" s="8"/>
@@ -2347,5 +2347,6 @@
     <hyperlink ref="I32" r:id="rId12" xr:uid="{EBC71EFF-54C7-3E4A-9B89-A57AAD183F48}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ajout de requêtes pour tester la base de données + informations
</commit_message>
<xml_diff>
--- a/bdd/infos_bdd.xlsx
+++ b/bdd/infos_bdd.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marieeonnet/Documents/Documents - MacBook Pro de Marie/Cours_DUT_Caen/Projet2A/dut2021_pret_instruments_voyage/bdd/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A06250C9-7DB9-444C-9E20-6E5CA9779B71}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE2B3E6D-264C-6B44-9C45-75977F4776A8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17020" yWindow="0" windowWidth="11780" windowHeight="18000" xr2:uid="{1C6F6E9A-B456-E643-B447-123029CC3B3E}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="19040" windowHeight="21600" xr2:uid="{1C6F6E9A-B456-E643-B447-123029CC3B3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="218">
-  <si>
-    <t>Vil_num</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="241">
   <si>
     <t>Vil_nom</t>
   </si>
@@ -688,13 +685,85 @@
   </si>
   <si>
     <t>clarinetDuet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requêtes </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Table </t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modifications </t>
+  </si>
+  <si>
+    <t>Instrument</t>
+  </si>
+  <si>
+    <t>Instrument dispo</t>
+  </si>
+  <si>
+    <t>SQL</t>
+  </si>
+  <si>
+    <t>Fonctionne correctement</t>
+  </si>
+  <si>
+    <t>select * from instrument join marque using(mar_numero);</t>
+  </si>
+  <si>
+    <t>select * from instrument join marque using(mar_numero) where mar_nom = 'Yamaha';</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jointure Instrument et Catégorie </t>
+  </si>
+  <si>
+    <t>seletc * from Instrument where ins_dipos = "oui";</t>
+  </si>
+  <si>
+    <t>select * from Instrument join Categorie using(cat_numero);</t>
+  </si>
+  <si>
+    <t>fonctionne correctement</t>
+  </si>
+  <si>
+    <t>Jointure Instrument et Marque</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jointure Instrument et Marque + nom marque </t>
+  </si>
+  <si>
+    <t>Jointure Instrument et Ville</t>
+  </si>
+  <si>
+    <t>Vil_numero</t>
+  </si>
+  <si>
+    <t>select * from Instrument join Ville using(vil_numero);</t>
+  </si>
+  <si>
+    <t>Jointure Instrument et utilisateur</t>
+  </si>
+  <si>
+    <t>select * from Instrument join Utilisateur using(uti_numero);</t>
+  </si>
+  <si>
+    <t>Instrument réserver par les utilisateurs</t>
+  </si>
+  <si>
+    <t>select * from Reserver join Utilisateur using(uti_numero) join Instrument using(ins_numero);</t>
+  </si>
+  <si>
+    <t>Peut être approfondie avec des where pour un utilisateur…</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -753,6 +822,27 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Courier New"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -762,7 +852,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -785,12 +875,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -832,6 +959,34 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1149,16 +1304,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D70755CD-10D4-DA48-863B-E92693C8657B}">
-  <dimension ref="B2:N46"/>
+  <dimension ref="B2:N81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I24" workbookViewId="0">
-      <selection activeCell="L46" sqref="L46"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="3" width="17.1640625" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="31.5" customWidth="1"/>
     <col min="5" max="5" width="17.1640625" customWidth="1"/>
     <col min="6" max="6" width="22.33203125" customWidth="1"/>
     <col min="7" max="7" width="20.83203125" customWidth="1"/>
@@ -1172,19 +1327,19 @@
   <sheetData>
     <row r="2" spans="2:6" ht="25" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="17" x14ac:dyDescent="0.2">
@@ -1192,16 +1347,16 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" s="1">
         <v>75001</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="17" x14ac:dyDescent="0.2">
@@ -1209,16 +1364,16 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" s="1">
         <v>13001</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="17" x14ac:dyDescent="0.2">
@@ -1226,16 +1381,16 @@
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" s="1">
         <v>59000</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="17" x14ac:dyDescent="0.2">
@@ -1243,16 +1398,16 @@
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" s="1">
         <v>33300</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="17" x14ac:dyDescent="0.2">
@@ -1260,16 +1415,16 @@
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" s="1">
         <v>61000</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="17" x14ac:dyDescent="0.2">
@@ -1277,16 +1432,16 @@
         <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8" s="1">
         <v>69000</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="17" x14ac:dyDescent="0.2">
@@ -1294,16 +1449,16 @@
         <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" s="1">
         <v>76620</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="17" x14ac:dyDescent="0.2">
@@ -1311,16 +1466,16 @@
         <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10" s="1">
         <v>21000</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="17" x14ac:dyDescent="0.2">
@@ -1328,16 +1483,16 @@
         <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" s="1">
         <v>87280</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="17" x14ac:dyDescent="0.2">
@@ -1345,16 +1500,16 @@
         <v>10</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D12" s="1">
         <v>35000</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="17" x14ac:dyDescent="0.2">
@@ -1362,16 +1517,16 @@
         <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D13" s="1">
         <v>14000</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="17" x14ac:dyDescent="0.2">
@@ -1379,16 +1534,16 @@
         <v>12</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D14" s="1">
         <v>14540</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="15" spans="2:6" ht="17" x14ac:dyDescent="0.2">
@@ -1396,16 +1551,16 @@
         <v>13</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D15" s="1">
         <v>27400</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="17" x14ac:dyDescent="0.2">
@@ -1413,13 +1568,13 @@
         <v>14</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D16" s="1">
         <v>76500</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F16" s="1">
         <v>1</v>
@@ -1430,16 +1585,16 @@
         <v>15</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D17" s="1">
         <v>64000</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="18" spans="2:14" ht="17" x14ac:dyDescent="0.2">
@@ -1447,16 +1602,16 @@
         <v>16</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D18" s="1">
         <v>17000</v>
       </c>
       <c r="E18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="19" spans="2:14" ht="17" x14ac:dyDescent="0.2">
@@ -1464,16 +1619,16 @@
         <v>17</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D19" s="1">
         <v>57050</v>
       </c>
       <c r="E19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="20" spans="2:14" ht="17" x14ac:dyDescent="0.2">
@@ -1481,16 +1636,16 @@
         <v>18</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D20" s="1">
         <v>54100</v>
       </c>
       <c r="E20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="21" spans="2:14" ht="17" x14ac:dyDescent="0.2">
@@ -1498,16 +1653,16 @@
         <v>19</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D21" s="1">
         <v>76100</v>
       </c>
       <c r="E21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="22" spans="2:14" ht="17" x14ac:dyDescent="0.2">
@@ -1515,16 +1670,16 @@
         <v>20</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D22" s="1">
         <v>30000</v>
       </c>
       <c r="E22" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.2">
@@ -1550,40 +1705,40 @@
     </row>
     <row r="26" spans="2:14" ht="22" x14ac:dyDescent="0.2">
       <c r="B26" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="D26" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="E26" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="F26" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="G26" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="G26" s="5" t="s">
+      <c r="H26" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="H26" s="5" t="s">
+      <c r="I26" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="I26" s="5" t="s">
+      <c r="J26" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="J26" s="5" t="s">
+      <c r="K26" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="K26" s="5" t="s">
+      <c r="L26" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="L26" s="5" t="s">
+      <c r="M26" s="5" t="s">
         <v>74</v>
-      </c>
-      <c r="M26" s="5" t="s">
-        <v>75</v>
       </c>
       <c r="N26" s="6"/>
     </row>
@@ -1595,13 +1750,13 @@
         <v>5</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E27" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="F27" s="8" t="s">
         <v>93</v>
-      </c>
-      <c r="F27" s="8" t="s">
-        <v>94</v>
       </c>
       <c r="G27" s="9">
         <v>37231</v>
@@ -1610,16 +1765,16 @@
         <v>44178</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J27" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="K27" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="L27" s="8" t="s">
         <v>214</v>
-      </c>
-      <c r="K27" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="L27" s="8" t="s">
-        <v>215</v>
       </c>
       <c r="M27" s="8"/>
       <c r="N27" s="8"/>
@@ -1632,31 +1787,31 @@
         <v>1</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E28" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F28" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="F28" s="8" t="s">
-        <v>98</v>
-      </c>
       <c r="G28" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H28" s="9">
         <v>44146</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="J28" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="K28" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="K28" s="8" t="s">
+      <c r="L28" s="13" t="s">
         <v>212</v>
-      </c>
-      <c r="L28" s="13" t="s">
-        <v>213</v>
       </c>
       <c r="M28" s="8"/>
       <c r="N28" s="8"/>
@@ -1669,13 +1824,13 @@
         <v>4</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E29" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="F29" s="8" t="s">
         <v>95</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>96</v>
       </c>
       <c r="G29" s="9">
         <v>37243</v>
@@ -1684,16 +1839,16 @@
         <v>43844</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J29" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="K29" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="K29" s="8" t="s">
+      <c r="L29" s="13" t="s">
         <v>209</v>
-      </c>
-      <c r="L29" s="13" t="s">
-        <v>210</v>
       </c>
       <c r="M29" s="8"/>
       <c r="N29" s="8"/>
@@ -1706,13 +1861,13 @@
         <v>10</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E30" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="F30" s="8" t="s">
         <v>100</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>101</v>
       </c>
       <c r="G30" s="9">
         <v>36588</v>
@@ -1721,16 +1876,16 @@
         <v>43893</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J30" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="K30" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="L30" s="13" t="s">
         <v>205</v>
-      </c>
-      <c r="K30" s="13" t="s">
-        <v>207</v>
-      </c>
-      <c r="L30" s="13" t="s">
-        <v>206</v>
       </c>
       <c r="M30" s="8"/>
       <c r="N30" s="8"/>
@@ -1743,13 +1898,13 @@
         <v>20</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E31" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="F31" s="8" t="s">
         <v>102</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>103</v>
       </c>
       <c r="G31" s="9">
         <v>37046</v>
@@ -1758,16 +1913,16 @@
         <v>43996</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="J31" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="K31" s="13" t="s">
         <v>202</v>
       </c>
-      <c r="K31" s="13" t="s">
+      <c r="L31" s="13" t="s">
         <v>203</v>
-      </c>
-      <c r="L31" s="13" t="s">
-        <v>204</v>
       </c>
       <c r="M31" s="8"/>
       <c r="N31" s="8"/>
@@ -1780,13 +1935,13 @@
         <v>6</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E32" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F32" s="8" t="s">
         <v>104</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>105</v>
       </c>
       <c r="G32" s="9">
         <v>36970</v>
@@ -1795,16 +1950,16 @@
         <v>44124</v>
       </c>
       <c r="I32" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="J32" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="J32" s="8" t="s">
+      <c r="K32" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="K32" s="8" t="s">
+      <c r="L32" s="13" t="s">
         <v>200</v>
-      </c>
-      <c r="L32" s="13" t="s">
-        <v>201</v>
       </c>
       <c r="M32" s="8"/>
       <c r="N32" s="8"/>
@@ -1817,13 +1972,13 @@
         <v>9</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E33" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="F33" s="8" t="s">
         <v>187</v>
-      </c>
-      <c r="F33" s="8" t="s">
-        <v>188</v>
       </c>
       <c r="G33" s="9">
         <v>36773</v>
@@ -1832,16 +1987,16 @@
         <v>44042</v>
       </c>
       <c r="I33" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="J33" s="13" t="s">
         <v>189</v>
       </c>
-      <c r="J33" s="13" t="s">
+      <c r="K33" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="K33" s="8" t="s">
+      <c r="L33" s="13" t="s">
         <v>191</v>
-      </c>
-      <c r="L33" s="13" t="s">
-        <v>192</v>
       </c>
       <c r="M33" s="8"/>
       <c r="N33" s="8"/>
@@ -1854,13 +2009,13 @@
         <v>11</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E34" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="F34" s="8" t="s">
         <v>107</v>
-      </c>
-      <c r="F34" s="8" t="s">
-        <v>108</v>
       </c>
       <c r="G34" s="9">
         <v>34095</v>
@@ -1869,16 +2024,16 @@
         <v>40533</v>
       </c>
       <c r="I34" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="J34" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="J34" s="12" t="s">
+      <c r="K34" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="L34" s="8" t="s">
         <v>110</v>
-      </c>
-      <c r="K34" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="L34" s="8" t="s">
-        <v>111</v>
       </c>
       <c r="M34" s="8"/>
       <c r="N34" s="8"/>
@@ -1891,13 +2046,13 @@
         <v>14</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E35" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="F35" s="8" t="s">
         <v>113</v>
-      </c>
-      <c r="F35" s="8" t="s">
-        <v>114</v>
       </c>
       <c r="G35" s="9">
         <v>27565</v>
@@ -1906,19 +2061,19 @@
         <v>40240</v>
       </c>
       <c r="I35" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="J35" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="J35" s="8" t="s">
+      <c r="K35" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="L35" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="K35" s="12" t="s">
+      <c r="M35" s="12" t="s">
         <v>118</v>
-      </c>
-      <c r="L35" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="M35" s="12" t="s">
-        <v>119</v>
       </c>
       <c r="N35" s="8"/>
     </row>
@@ -1930,13 +2085,13 @@
         <v>15</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E36" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="F36" s="8" t="s">
         <v>120</v>
-      </c>
-      <c r="F36" s="8" t="s">
-        <v>121</v>
       </c>
       <c r="G36" s="9">
         <v>26789</v>
@@ -1945,16 +2100,16 @@
         <v>40933</v>
       </c>
       <c r="I36" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="J36" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="J36" s="8" t="s">
+      <c r="K36" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="L36" s="13" t="s">
         <v>123</v>
-      </c>
-      <c r="K36" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="L36" s="13" t="s">
-        <v>124</v>
       </c>
       <c r="M36" s="8"/>
       <c r="N36" s="8"/>
@@ -1967,13 +2122,13 @@
         <v>19</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E37" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="F37" s="8" t="s">
         <v>126</v>
-      </c>
-      <c r="F37" s="8" t="s">
-        <v>127</v>
       </c>
       <c r="G37" s="9">
         <v>29468</v>
@@ -1982,16 +2137,16 @@
         <v>39913</v>
       </c>
       <c r="I37" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="J37" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="J37" s="13" t="s">
+      <c r="K37" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="K37" s="13" t="s">
+      <c r="L37" s="13" t="s">
         <v>130</v>
-      </c>
-      <c r="L37" s="13" t="s">
-        <v>131</v>
       </c>
       <c r="M37" s="8"/>
       <c r="N37" s="8"/>
@@ -2004,13 +2159,13 @@
         <v>2</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G38" s="9">
         <v>28337</v>
@@ -2019,16 +2174,16 @@
         <v>40179</v>
       </c>
       <c r="I38" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="J38" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="J38" s="13" t="s">
+      <c r="K38" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="L38" s="13" t="s">
         <v>134</v>
-      </c>
-      <c r="K38" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="L38" s="13" t="s">
-        <v>135</v>
       </c>
       <c r="M38" s="8"/>
       <c r="N38" s="8"/>
@@ -2041,13 +2196,13 @@
         <v>3</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E39" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="F39" s="8" t="s">
         <v>137</v>
-      </c>
-      <c r="F39" s="8" t="s">
-        <v>138</v>
       </c>
       <c r="G39" s="9">
         <v>27435</v>
@@ -2056,16 +2211,16 @@
         <v>41917</v>
       </c>
       <c r="I39" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="J39" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="J39" s="13" t="s">
+      <c r="K39" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="L39" s="13" t="s">
         <v>140</v>
-      </c>
-      <c r="K39" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="L39" s="13" t="s">
-        <v>141</v>
       </c>
       <c r="M39" s="8"/>
       <c r="N39" s="8"/>
@@ -2078,13 +2233,13 @@
         <v>7</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E40" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="F40" s="8" t="s">
         <v>143</v>
-      </c>
-      <c r="F40" s="8" t="s">
-        <v>144</v>
       </c>
       <c r="G40" s="9">
         <v>31859</v>
@@ -2093,16 +2248,16 @@
         <v>40362</v>
       </c>
       <c r="I40" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="J40" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="K40" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="L40" s="13" t="s">
         <v>145</v>
-      </c>
-      <c r="J40" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="K40" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="L40" s="13" t="s">
-        <v>146</v>
       </c>
       <c r="M40" s="8"/>
       <c r="N40" s="8"/>
@@ -2115,13 +2270,13 @@
         <v>8</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E41" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="F41" s="8" t="s">
         <v>149</v>
-      </c>
-      <c r="F41" s="8" t="s">
-        <v>150</v>
       </c>
       <c r="G41" s="14">
         <v>28506</v>
@@ -2130,16 +2285,16 @@
         <v>42368</v>
       </c>
       <c r="I41" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="J41" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="J41" s="13" t="s">
+      <c r="K41" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="L41" s="13" t="s">
         <v>152</v>
-      </c>
-      <c r="K41" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="L41" s="13" t="s">
-        <v>153</v>
       </c>
       <c r="M41" s="8"/>
       <c r="N41" s="8"/>
@@ -2152,13 +2307,13 @@
         <v>13</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E42" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="F42" s="8" t="s">
         <v>155</v>
-      </c>
-      <c r="F42" s="8" t="s">
-        <v>156</v>
       </c>
       <c r="G42" s="9">
         <v>26846</v>
@@ -2167,16 +2322,16 @@
         <v>44177</v>
       </c>
       <c r="I42" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="J42" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="J42" s="13" t="s">
+      <c r="K42" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="L42" s="13" t="s">
         <v>158</v>
-      </c>
-      <c r="K42" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="L42" s="13" t="s">
-        <v>159</v>
       </c>
       <c r="M42" s="8"/>
       <c r="N42" s="8"/>
@@ -2189,13 +2344,13 @@
         <v>12</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E43" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="F43" s="8" t="s">
         <v>161</v>
-      </c>
-      <c r="F43" s="8" t="s">
-        <v>162</v>
       </c>
       <c r="G43" s="9">
         <v>33439</v>
@@ -2204,19 +2359,19 @@
         <v>43047</v>
       </c>
       <c r="I43" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="J43" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="J43" s="8" t="s">
+      <c r="K43" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="K43" s="8" t="s">
+      <c r="L43" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="L43" s="13" t="s">
+      <c r="M43" s="13" t="s">
         <v>166</v>
-      </c>
-      <c r="M43" s="13" t="s">
-        <v>167</v>
       </c>
       <c r="N43" s="8"/>
     </row>
@@ -2228,13 +2383,13 @@
         <v>16</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E44" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="F44" s="11" t="s">
         <v>168</v>
-      </c>
-      <c r="F44" s="11" t="s">
-        <v>169</v>
       </c>
       <c r="G44" s="9">
         <v>28991</v>
@@ -2243,16 +2398,16 @@
         <v>41517</v>
       </c>
       <c r="I44" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="J44" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="J44" s="8" t="s">
+      <c r="K44" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="K44" s="8" t="s">
+      <c r="L44" s="13" t="s">
         <v>172</v>
-      </c>
-      <c r="L44" s="13" t="s">
-        <v>173</v>
       </c>
       <c r="M44" s="8"/>
       <c r="N44" s="8"/>
@@ -2265,13 +2420,13 @@
         <v>18</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E45" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="F45" s="8" t="s">
         <v>174</v>
-      </c>
-      <c r="F45" s="8" t="s">
-        <v>175</v>
       </c>
       <c r="G45" s="9">
         <v>34480</v>
@@ -2280,16 +2435,16 @@
         <v>43748</v>
       </c>
       <c r="I45" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="J45" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="J45" s="13" t="s">
+      <c r="K45" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="K45" s="8" t="s">
+      <c r="L45" s="13" t="s">
         <v>178</v>
-      </c>
-      <c r="L45" s="13" t="s">
-        <v>179</v>
       </c>
       <c r="M45" s="8"/>
       <c r="N45" s="8"/>
@@ -2302,13 +2457,13 @@
         <v>17</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E46" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="F46" s="8" t="s">
         <v>180</v>
-      </c>
-      <c r="F46" s="8" t="s">
-        <v>181</v>
       </c>
       <c r="G46" s="9">
         <v>36294</v>
@@ -2317,21 +2472,295 @@
         <v>43966</v>
       </c>
       <c r="I46" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="J46" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="J46" s="8" t="s">
+      <c r="K46" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="L46" s="13" t="s">
         <v>183</v>
-      </c>
-      <c r="K46" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="L46" s="13" t="s">
-        <v>184</v>
       </c>
       <c r="M46" s="8"/>
       <c r="N46" s="8"/>
     </row>
+    <row r="50" spans="2:6" ht="21" x14ac:dyDescent="0.25">
+      <c r="B50" s="15" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="B52" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="C52" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="D52" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="E52" s="16" t="s">
+        <v>220</v>
+      </c>
+      <c r="F52" s="16" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="B53" s="18" t="s">
+        <v>221</v>
+      </c>
+      <c r="C53" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="D53" s="23" t="s">
+        <v>228</v>
+      </c>
+      <c r="E53" s="17"/>
+      <c r="F53" s="17" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" ht="54" x14ac:dyDescent="0.25">
+      <c r="B54" s="19"/>
+      <c r="C54" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="D54" s="23" t="s">
+        <v>225</v>
+      </c>
+      <c r="E54" s="17"/>
+      <c r="F54" s="17" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" ht="72" x14ac:dyDescent="0.25">
+      <c r="B55" s="19"/>
+      <c r="C55" s="17" t="s">
+        <v>232</v>
+      </c>
+      <c r="D55" s="23" t="s">
+        <v>226</v>
+      </c>
+      <c r="E55" s="17"/>
+      <c r="F55" s="17" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" ht="54" x14ac:dyDescent="0.25">
+      <c r="B56" s="19"/>
+      <c r="C56" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="D56" s="23" t="s">
+        <v>229</v>
+      </c>
+      <c r="E56" s="17"/>
+      <c r="F56" s="17" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" ht="54" x14ac:dyDescent="0.25">
+      <c r="B57" s="19"/>
+      <c r="C57" s="17" t="s">
+        <v>233</v>
+      </c>
+      <c r="D57" s="24" t="s">
+        <v>235</v>
+      </c>
+      <c r="E57" s="17"/>
+      <c r="F57" s="17" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" ht="54" x14ac:dyDescent="0.25">
+      <c r="B58" s="19"/>
+      <c r="C58" s="22" t="s">
+        <v>236</v>
+      </c>
+      <c r="D58" s="23" t="s">
+        <v>237</v>
+      </c>
+      <c r="E58" s="17"/>
+      <c r="F58" s="17" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="B59" s="19"/>
+      <c r="C59" s="17" t="s">
+        <v>238</v>
+      </c>
+      <c r="D59" s="23" t="s">
+        <v>239</v>
+      </c>
+      <c r="E59" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="F59" s="17" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="B60" s="19"/>
+      <c r="C60" s="17"/>
+      <c r="D60" s="23"/>
+      <c r="E60" s="17"/>
+      <c r="F60" s="17"/>
+    </row>
+    <row r="61" spans="2:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="B61" s="20"/>
+      <c r="C61" s="17"/>
+      <c r="D61" s="23"/>
+      <c r="E61" s="17"/>
+      <c r="F61" s="17"/>
+    </row>
+    <row r="62" spans="2:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="B62" s="17"/>
+      <c r="C62" s="17"/>
+      <c r="D62" s="23"/>
+      <c r="E62" s="17"/>
+      <c r="F62" s="17"/>
+    </row>
+    <row r="63" spans="2:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="B63" s="17"/>
+      <c r="C63" s="17"/>
+      <c r="D63" s="23"/>
+      <c r="E63" s="17"/>
+      <c r="F63" s="17"/>
+    </row>
+    <row r="64" spans="2:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="B64" s="17"/>
+      <c r="C64" s="17"/>
+      <c r="D64" s="23"/>
+      <c r="E64" s="17"/>
+      <c r="F64" s="17"/>
+    </row>
+    <row r="65" spans="2:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="B65" s="17"/>
+      <c r="C65" s="17"/>
+      <c r="D65" s="23"/>
+      <c r="E65" s="17"/>
+      <c r="F65" s="17"/>
+    </row>
+    <row r="66" spans="2:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="B66" s="17"/>
+      <c r="C66" s="17"/>
+      <c r="D66" s="23"/>
+      <c r="E66" s="17"/>
+      <c r="F66" s="17"/>
+    </row>
+    <row r="67" spans="2:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="B67" s="17"/>
+      <c r="C67" s="17"/>
+      <c r="D67" s="23"/>
+      <c r="E67" s="17"/>
+      <c r="F67" s="17"/>
+    </row>
+    <row r="68" spans="2:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="B68" s="17"/>
+      <c r="C68" s="17"/>
+      <c r="D68" s="23"/>
+      <c r="E68" s="17"/>
+      <c r="F68" s="17"/>
+    </row>
+    <row r="69" spans="2:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="B69" s="17"/>
+      <c r="C69" s="17"/>
+      <c r="D69" s="23"/>
+      <c r="E69" s="17"/>
+      <c r="F69" s="17"/>
+    </row>
+    <row r="70" spans="2:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="B70" s="17"/>
+      <c r="C70" s="17"/>
+      <c r="D70" s="23"/>
+      <c r="E70" s="17"/>
+      <c r="F70" s="17"/>
+    </row>
+    <row r="71" spans="2:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="B71" s="17"/>
+      <c r="C71" s="17"/>
+      <c r="D71" s="23"/>
+      <c r="E71" s="17"/>
+      <c r="F71" s="17"/>
+    </row>
+    <row r="72" spans="2:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="B72" s="17"/>
+      <c r="C72" s="17"/>
+      <c r="D72" s="23"/>
+      <c r="E72" s="17"/>
+      <c r="F72" s="17"/>
+    </row>
+    <row r="73" spans="2:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="B73" s="17"/>
+      <c r="C73" s="17"/>
+      <c r="D73" s="23"/>
+      <c r="E73" s="17"/>
+      <c r="F73" s="17"/>
+    </row>
+    <row r="74" spans="2:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="B74" s="17"/>
+      <c r="C74" s="17"/>
+      <c r="D74" s="23"/>
+      <c r="E74" s="17"/>
+      <c r="F74" s="17"/>
+    </row>
+    <row r="75" spans="2:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="B75" s="17"/>
+      <c r="C75" s="17"/>
+      <c r="D75" s="23"/>
+      <c r="E75" s="17"/>
+      <c r="F75" s="17"/>
+    </row>
+    <row r="76" spans="2:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="B76" s="17"/>
+      <c r="C76" s="17"/>
+      <c r="D76" s="23"/>
+      <c r="E76" s="17"/>
+      <c r="F76" s="17"/>
+    </row>
+    <row r="77" spans="2:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="B77" s="17"/>
+      <c r="C77" s="17"/>
+      <c r="D77" s="23"/>
+      <c r="E77" s="17"/>
+      <c r="F77" s="17"/>
+    </row>
+    <row r="78" spans="2:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="B78" s="17"/>
+      <c r="C78" s="17"/>
+      <c r="D78" s="23"/>
+      <c r="E78" s="17"/>
+      <c r="F78" s="17"/>
+    </row>
+    <row r="79" spans="2:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="B79" s="17"/>
+      <c r="C79" s="17"/>
+      <c r="D79" s="23"/>
+      <c r="E79" s="17"/>
+      <c r="F79" s="17"/>
+    </row>
+    <row r="80" spans="2:6" ht="17" x14ac:dyDescent="0.25">
+      <c r="B80" s="17"/>
+      <c r="C80" s="17"/>
+      <c r="D80" s="23"/>
+      <c r="E80" s="17"/>
+      <c r="F80" s="17"/>
+    </row>
+    <row r="81" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B81" s="21"/>
+      <c r="C81" s="21"/>
+      <c r="D81" s="21"/>
+      <c r="E81" s="21"/>
+      <c r="F81" s="21"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B53:B61"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="I34" r:id="rId1" xr:uid="{BA1FB798-E09E-724C-B38A-559701AF93EA}"/>
     <hyperlink ref="I35" r:id="rId2" xr:uid="{0A154888-FD69-F744-9B89-4A33C50548E0}"/>

</xml_diff>

<commit_message>
modif type char en date pour table Message et ajout de requêtes de tests
</commit_message>
<xml_diff>
--- a/bdd/infos_bdd.xlsx
+++ b/bdd/infos_bdd.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marieeonnet/Documents/Documents - MacBook Pro de Marie/Cours_DUT_Caen/Projet2A/dut2021_pret_instruments_voyage/bdd/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE2B3E6D-264C-6B44-9C45-75977F4776A8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{087392BF-0491-4945-BB88-D1D7E73E0179}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="0" windowWidth="19040" windowHeight="21600" xr2:uid="{1C6F6E9A-B456-E643-B447-123029CC3B3E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="249">
   <si>
     <t>Vil_nom</t>
   </si>
@@ -690,9 +690,6 @@
     <t xml:space="preserve">Requêtes </t>
   </si>
   <si>
-    <t xml:space="preserve">Table </t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -757,13 +754,40 @@
   </si>
   <si>
     <t>Peut être approfondie avec des where pour un utilisateur…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intrument représenté par une image </t>
+  </si>
+  <si>
+    <t>select * from representer joi Instrument using(ins_numero) join image(ima_num);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utilisateur </t>
+  </si>
+  <si>
+    <t>Tables</t>
+  </si>
+  <si>
+    <t>Jointure Utilisateur et Ville</t>
+  </si>
+  <si>
+    <t>select * from Utilisateur join Ville using(vil_numero);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jointure Utilisateur et Message </t>
+  </si>
+  <si>
+    <t>select * from Utilisateur join Message using(uti_numero)</t>
+  </si>
+  <si>
+    <t>Modification du type char en date pour msg_date_envoi et msg_date_ouverture pour la table Message</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -833,13 +857,6 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Courier New"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Courier New"/>
       <family val="1"/>
     </font>
@@ -986,7 +1003,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1306,8 +1323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D70755CD-10D4-DA48-863B-E92693C8657B}">
   <dimension ref="B2:N81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="G59" sqref="G59"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1327,7 +1344,7 @@
   <sheetData>
     <row r="2" spans="2:6" ht="25" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>0</v>
@@ -2493,122 +2510,128 @@
     </row>
     <row r="52" spans="2:6" ht="17" x14ac:dyDescent="0.2">
       <c r="B52" s="16" t="s">
-        <v>218</v>
+        <v>243</v>
       </c>
       <c r="C52" s="16" t="s">
         <v>217</v>
       </c>
       <c r="D52" s="16" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E52" s="16" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F52" s="16" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="53" spans="2:6" ht="36" x14ac:dyDescent="0.25">
       <c r="B53" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="C53" s="17" t="s">
         <v>221</v>
       </c>
-      <c r="C53" s="17" t="s">
-        <v>222</v>
-      </c>
       <c r="D53" s="23" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E53" s="17"/>
       <c r="F53" s="17" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="54" spans="2:6" ht="54" x14ac:dyDescent="0.25">
       <c r="B54" s="19"/>
       <c r="C54" s="17" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D54" s="23" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E54" s="17"/>
       <c r="F54" s="17" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="55" spans="2:6" ht="72" x14ac:dyDescent="0.25">
       <c r="B55" s="19"/>
       <c r="C55" s="17" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D55" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E55" s="17"/>
       <c r="F55" s="17" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="56" spans="2:6" ht="54" x14ac:dyDescent="0.25">
       <c r="B56" s="19"/>
       <c r="C56" s="17" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D56" s="23" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E56" s="17"/>
       <c r="F56" s="17" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="57" spans="2:6" ht="54" x14ac:dyDescent="0.25">
       <c r="B57" s="19"/>
       <c r="C57" s="17" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D57" s="24" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E57" s="17"/>
       <c r="F57" s="17" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="58" spans="2:6" ht="54" x14ac:dyDescent="0.25">
       <c r="B58" s="19"/>
       <c r="C58" s="22" t="s">
+        <v>235</v>
+      </c>
+      <c r="D58" s="23" t="s">
         <v>236</v>
-      </c>
-      <c r="D58" s="23" t="s">
-        <v>237</v>
       </c>
       <c r="E58" s="17"/>
       <c r="F58" s="17" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="59" spans="2:6" ht="90" x14ac:dyDescent="0.25">
       <c r="B59" s="19"/>
       <c r="C59" s="17" t="s">
+        <v>237</v>
+      </c>
+      <c r="D59" s="23" t="s">
         <v>238</v>
       </c>
-      <c r="D59" s="23" t="s">
+      <c r="E59" s="17" t="s">
         <v>239</v>
       </c>
-      <c r="E59" s="17" t="s">
+      <c r="F59" s="17" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" ht="72" x14ac:dyDescent="0.25">
+      <c r="B60" s="19"/>
+      <c r="C60" s="17" t="s">
         <v>240</v>
       </c>
-      <c r="F59" s="17" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="60" spans="2:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="B60" s="19"/>
-      <c r="C60" s="17"/>
-      <c r="D60" s="23"/>
+      <c r="D60" s="23" t="s">
+        <v>241</v>
+      </c>
       <c r="E60" s="17"/>
-      <c r="F60" s="17"/>
+      <c r="F60" s="17" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="61" spans="2:6" ht="17" x14ac:dyDescent="0.25">
       <c r="B61" s="20"/>
@@ -2617,57 +2640,73 @@
       <c r="E61" s="17"/>
       <c r="F61" s="17"/>
     </row>
-    <row r="62" spans="2:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="B62" s="17"/>
-      <c r="C62" s="17"/>
-      <c r="D62" s="23"/>
+    <row r="62" spans="2:6" ht="54" x14ac:dyDescent="0.25">
+      <c r="B62" s="18" t="s">
+        <v>242</v>
+      </c>
+      <c r="C62" s="17" t="s">
+        <v>244</v>
+      </c>
+      <c r="D62" s="23" t="s">
+        <v>245</v>
+      </c>
       <c r="E62" s="17"/>
-      <c r="F62" s="17"/>
-    </row>
-    <row r="63" spans="2:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="B63" s="17"/>
-      <c r="C63" s="17"/>
-      <c r="D63" s="23"/>
-      <c r="E63" s="17"/>
-      <c r="F63" s="17"/>
+      <c r="F62" s="17" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="B63" s="19"/>
+      <c r="C63" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="D63" s="23" t="s">
+        <v>247</v>
+      </c>
+      <c r="E63" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="F63" s="17" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="64" spans="2:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="B64" s="17"/>
+      <c r="B64" s="19"/>
       <c r="C64" s="17"/>
       <c r="D64" s="23"/>
       <c r="E64" s="17"/>
       <c r="F64" s="17"/>
     </row>
     <row r="65" spans="2:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="B65" s="17"/>
+      <c r="B65" s="19"/>
       <c r="C65" s="17"/>
       <c r="D65" s="23"/>
       <c r="E65" s="17"/>
       <c r="F65" s="17"/>
     </row>
     <row r="66" spans="2:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="B66" s="17"/>
+      <c r="B66" s="19"/>
       <c r="C66" s="17"/>
       <c r="D66" s="23"/>
       <c r="E66" s="17"/>
       <c r="F66" s="17"/>
     </row>
     <row r="67" spans="2:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="B67" s="17"/>
+      <c r="B67" s="19"/>
       <c r="C67" s="17"/>
       <c r="D67" s="23"/>
       <c r="E67" s="17"/>
       <c r="F67" s="17"/>
     </row>
     <row r="68" spans="2:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="B68" s="17"/>
+      <c r="B68" s="19"/>
       <c r="C68" s="17"/>
       <c r="D68" s="23"/>
       <c r="E68" s="17"/>
       <c r="F68" s="17"/>
     </row>
     <row r="69" spans="2:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="B69" s="17"/>
+      <c r="B69" s="20"/>
       <c r="C69" s="17"/>
       <c r="D69" s="23"/>
       <c r="E69" s="17"/>
@@ -2758,8 +2797,9 @@
       <c r="F81" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B53:B61"/>
+    <mergeCell ref="B62:B69"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I34" r:id="rId1" xr:uid="{BA1FB798-E09E-724C-B38A-559701AF93EA}"/>

</xml_diff>

<commit_message>
ajout des nouvelles infos insérées dans la base
</commit_message>
<xml_diff>
--- a/bdd/infos_bdd.xlsx
+++ b/bdd/infos_bdd.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marieeonnet/Documents/Documents - MacBook Pro de Marie/Cours_DUT_Caen/Projet2A/dut2021_pret_instruments_voyage/bdd/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{087392BF-0491-4945-BB88-D1D7E73E0179}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB53432-AE3F-7841-B70E-557690525DE7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="19040" windowHeight="21600" xr2:uid="{1C6F6E9A-B456-E643-B447-123029CC3B3E}"/>
+    <workbookView xWindow="880" yWindow="500" windowWidth="24380" windowHeight="17020" xr2:uid="{1C6F6E9A-B456-E643-B447-123029CC3B3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="315">
   <si>
     <t>Vil_nom</t>
   </si>
@@ -781,6 +781,204 @@
   </si>
   <si>
     <t>Modification du type char en date pour msg_date_envoi et msg_date_ouverture pour la table Message</t>
+  </si>
+  <si>
+    <t>Ville</t>
+  </si>
+  <si>
+    <t>Utilisateur</t>
+  </si>
+  <si>
+    <t>Marques</t>
+  </si>
+  <si>
+    <t>MAR_NUMERO</t>
+  </si>
+  <si>
+    <t>MAR_NOM</t>
+  </si>
+  <si>
+    <t>MAR_DATE_AJOUT</t>
+  </si>
+  <si>
+    <t>Bergerault</t>
+  </si>
+  <si>
+    <t>Yamaha</t>
+  </si>
+  <si>
+    <t>Pearl</t>
+  </si>
+  <si>
+    <t>DW</t>
+  </si>
+  <si>
+    <t>Bach</t>
+  </si>
+  <si>
+    <t>Fender</t>
+  </si>
+  <si>
+    <t>Gibson</t>
+  </si>
+  <si>
+    <t>Gretsch</t>
+  </si>
+  <si>
+    <t>Kawai</t>
+  </si>
+  <si>
+    <t>Paul Red Smith</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instruments </t>
+  </si>
+  <si>
+    <t>INS_NUMERO</t>
+  </si>
+  <si>
+    <t>VIL_NUMERO</t>
+  </si>
+  <si>
+    <t>UTI_NUMERO</t>
+  </si>
+  <si>
+    <t>CAT_NUMERO</t>
+  </si>
+  <si>
+    <t>INS_NOM</t>
+  </si>
+  <si>
+    <t>INS_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>INS_DISPONIBLE</t>
+  </si>
+  <si>
+    <t>IN_DATE_AJOUT</t>
+  </si>
+  <si>
+    <t>INS_PRIX</t>
+  </si>
+  <si>
+    <t>INS_PHOTO</t>
+  </si>
+  <si>
+    <t>Marimba(4 octaves)</t>
+  </si>
+  <si>
+    <t>Batterie DW</t>
+  </si>
+  <si>
+    <t>Cor d'harmonie</t>
+  </si>
+  <si>
+    <t>Squier Bullet Strat HSS BSB</t>
+  </si>
+  <si>
+    <t>PRS SE P20E Parlor PB LTD</t>
+  </si>
+  <si>
+    <t>ES-110 B</t>
+  </si>
+  <si>
+    <t>YCL-457II-22 Clarinet</t>
+  </si>
+  <si>
+    <t>oui</t>
+  </si>
+  <si>
+    <t>99.99</t>
+  </si>
+  <si>
+    <t>Catégorie</t>
+  </si>
+  <si>
+    <t>CAT_NOM</t>
+  </si>
+  <si>
+    <t>CAT_FAMILLE</t>
+  </si>
+  <si>
+    <t>Batterie</t>
+  </si>
+  <si>
+    <t>Marimba</t>
+  </si>
+  <si>
+    <t>Xylophone</t>
+  </si>
+  <si>
+    <t>Timbales</t>
+  </si>
+  <si>
+    <t>Tambour</t>
+  </si>
+  <si>
+    <t>Trompette</t>
+  </si>
+  <si>
+    <t>Trombonne</t>
+  </si>
+  <si>
+    <t>Euphonium</t>
+  </si>
+  <si>
+    <t>Clarinette</t>
+  </si>
+  <si>
+    <t>Guitare Electrique</t>
+  </si>
+  <si>
+    <t>Guitare Classique</t>
+  </si>
+  <si>
+    <t>Guitare Folk</t>
+  </si>
+  <si>
+    <t>Piano Numérique</t>
+  </si>
+  <si>
+    <t>Percussions</t>
+  </si>
+  <si>
+    <t>Cuivres</t>
+  </si>
+  <si>
+    <t>Vent</t>
+  </si>
+  <si>
+    <t>Guitare</t>
+  </si>
+  <si>
+    <t>Clavier</t>
+  </si>
+  <si>
+    <t>Cordes</t>
+  </si>
+  <si>
+    <t>Cordes pincées</t>
+  </si>
+  <si>
+    <t>Cordes frottées</t>
+  </si>
+  <si>
+    <t>Pouces</t>
+  </si>
+  <si>
+    <t>Kalimba 17 touches</t>
+  </si>
+  <si>
+    <t>Gear4music</t>
+  </si>
+  <si>
+    <t>Harpe 12 cordes</t>
+  </si>
+  <si>
+    <t>Harpe</t>
+  </si>
+  <si>
+    <t>Piano</t>
   </si>
 </sst>
 </file>
@@ -869,7 +1067,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -929,12 +1127,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -985,15 +1192,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1005,6 +1203,45 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1321,10 +1558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D70755CD-10D4-DA48-863B-E92693C8657B}">
-  <dimension ref="B2:N81"/>
+  <dimension ref="A2:V81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="F64" sqref="F64"/>
+    <sheetView tabSelected="1" topLeftCell="M4" workbookViewId="0">
+      <selection activeCell="U27" sqref="U27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1336,13 +1573,24 @@
     <col min="7" max="7" width="20.83203125" customWidth="1"/>
     <col min="8" max="8" width="26.6640625" customWidth="1"/>
     <col min="9" max="9" width="37.6640625" customWidth="1"/>
-    <col min="10" max="10" width="15.83203125" customWidth="1"/>
+    <col min="10" max="10" width="18" customWidth="1"/>
     <col min="11" max="11" width="22.6640625" customWidth="1"/>
-    <col min="12" max="12" width="17.6640625" customWidth="1"/>
-    <col min="13" max="13" width="19.5" customWidth="1"/>
+    <col min="12" max="13" width="24.33203125" customWidth="1"/>
+    <col min="14" max="14" width="15.5" customWidth="1"/>
+    <col min="15" max="15" width="15.6640625" customWidth="1"/>
+    <col min="16" max="16" width="17.6640625" customWidth="1"/>
+    <col min="17" max="17" width="16.83203125" customWidth="1"/>
+    <col min="18" max="18" width="17.1640625" customWidth="1"/>
+    <col min="19" max="19" width="15.1640625" customWidth="1"/>
+    <col min="20" max="20" width="19.1640625" customWidth="1"/>
+    <col min="21" max="21" width="17" customWidth="1"/>
+    <col min="22" max="22" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" ht="50" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>249</v>
+      </c>
       <c r="B2" s="2" t="s">
         <v>233</v>
       </c>
@@ -1358,8 +1606,56 @@
       <c r="F2" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="G2" s="25" t="s">
+        <v>251</v>
+      </c>
+      <c r="H2" s="26" t="s">
+        <v>252</v>
+      </c>
+      <c r="I2" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="J2" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="K2" s="28" t="s">
+        <v>265</v>
+      </c>
+      <c r="L2" s="26" t="s">
+        <v>266</v>
+      </c>
+      <c r="M2" s="26" t="s">
+        <v>252</v>
+      </c>
+      <c r="N2" s="26" t="s">
+        <v>267</v>
+      </c>
+      <c r="O2" s="26" t="s">
+        <v>268</v>
+      </c>
+      <c r="P2" s="26" t="s">
+        <v>269</v>
+      </c>
+      <c r="Q2" s="26" t="s">
+        <v>270</v>
+      </c>
+      <c r="R2" s="26" t="s">
+        <v>271</v>
+      </c>
+      <c r="S2" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="T2" s="26" t="s">
+        <v>273</v>
+      </c>
+      <c r="U2" s="26" t="s">
+        <v>274</v>
+      </c>
+      <c r="V2" s="26" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" ht="34" x14ac:dyDescent="0.2">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -1375,8 +1671,46 @@
       <c r="F3" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="H3" s="6">
+        <v>1</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="J3" s="27">
+        <v>44195</v>
+      </c>
+      <c r="L3" s="30">
+        <v>1</v>
+      </c>
+      <c r="M3" s="30">
+        <v>1</v>
+      </c>
+      <c r="N3" s="30">
+        <v>1</v>
+      </c>
+      <c r="O3" s="30">
+        <v>1</v>
+      </c>
+      <c r="P3" s="30">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="30" t="s">
+        <v>276</v>
+      </c>
+      <c r="R3" s="30"/>
+      <c r="S3" s="30" t="s">
+        <v>283</v>
+      </c>
+      <c r="T3" s="31">
+        <v>44203</v>
+      </c>
+      <c r="U3" s="30">
+        <v>0</v>
+      </c>
+      <c r="V3" s="30"/>
+    </row>
+    <row r="4" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="B4" s="1">
         <v>2</v>
       </c>
@@ -1392,8 +1726,46 @@
       <c r="F4" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="H4" s="6">
+        <v>2</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="J4" s="27">
+        <v>44195</v>
+      </c>
+      <c r="L4" s="30">
+        <v>2</v>
+      </c>
+      <c r="M4" s="30">
+        <v>4</v>
+      </c>
+      <c r="N4" s="30">
+        <v>4</v>
+      </c>
+      <c r="O4" s="30">
+        <v>4</v>
+      </c>
+      <c r="P4" s="30">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="30" t="s">
+        <v>277</v>
+      </c>
+      <c r="R4" s="30"/>
+      <c r="S4" s="30" t="s">
+        <v>283</v>
+      </c>
+      <c r="T4" s="31">
+        <v>44195</v>
+      </c>
+      <c r="U4" s="30">
+        <v>99</v>
+      </c>
+      <c r="V4" s="30"/>
+    </row>
+    <row r="5" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="B5" s="1">
         <v>3</v>
       </c>
@@ -1409,8 +1781,46 @@
       <c r="F5" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="H5" s="6">
+        <v>3</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="J5" s="27">
+        <v>44195</v>
+      </c>
+      <c r="L5" s="30">
+        <v>3</v>
+      </c>
+      <c r="M5" s="30">
+        <v>2</v>
+      </c>
+      <c r="N5" s="30">
+        <v>18</v>
+      </c>
+      <c r="O5" s="30">
+        <v>15</v>
+      </c>
+      <c r="P5" s="30">
+        <v>9</v>
+      </c>
+      <c r="Q5" s="30" t="s">
+        <v>278</v>
+      </c>
+      <c r="R5" s="30"/>
+      <c r="S5" s="30" t="s">
+        <v>283</v>
+      </c>
+      <c r="T5" s="31">
+        <v>44203</v>
+      </c>
+      <c r="U5" s="30">
+        <v>0</v>
+      </c>
+      <c r="V5" s="30"/>
+    </row>
+    <row r="6" spans="1:22" ht="34" x14ac:dyDescent="0.2">
       <c r="B6" s="1">
         <v>4</v>
       </c>
@@ -1426,8 +1836,46 @@
       <c r="F6" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="H6" s="6">
+        <v>4</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="J6" s="27">
+        <v>44195</v>
+      </c>
+      <c r="L6" s="30">
+        <v>4</v>
+      </c>
+      <c r="M6" s="30">
+        <v>6</v>
+      </c>
+      <c r="N6" s="30">
+        <v>13</v>
+      </c>
+      <c r="O6" s="30">
+        <v>18</v>
+      </c>
+      <c r="P6" s="30">
+        <v>11</v>
+      </c>
+      <c r="Q6" s="30" t="s">
+        <v>279</v>
+      </c>
+      <c r="R6" s="30"/>
+      <c r="S6" s="30" t="s">
+        <v>283</v>
+      </c>
+      <c r="T6" s="31">
+        <v>44195</v>
+      </c>
+      <c r="U6" s="30">
+        <v>10</v>
+      </c>
+      <c r="V6" s="30"/>
+    </row>
+    <row r="7" spans="1:22" ht="34" x14ac:dyDescent="0.2">
       <c r="B7" s="1">
         <v>5</v>
       </c>
@@ -1443,8 +1891,46 @@
       <c r="F7" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="H7" s="6">
+        <v>5</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="J7" s="27">
+        <v>44195</v>
+      </c>
+      <c r="L7" s="30">
+        <v>5</v>
+      </c>
+      <c r="M7" s="30">
+        <v>10</v>
+      </c>
+      <c r="N7" s="30">
+        <v>19</v>
+      </c>
+      <c r="O7" s="30">
+        <v>22</v>
+      </c>
+      <c r="P7" s="30">
+        <v>13</v>
+      </c>
+      <c r="Q7" s="30" t="s">
+        <v>280</v>
+      </c>
+      <c r="R7" s="30"/>
+      <c r="S7" s="30" t="s">
+        <v>283</v>
+      </c>
+      <c r="T7" s="31">
+        <v>44203</v>
+      </c>
+      <c r="U7" s="30">
+        <v>0</v>
+      </c>
+      <c r="V7" s="30"/>
+    </row>
+    <row r="8" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" s="1">
         <v>6</v>
       </c>
@@ -1460,8 +1946,46 @@
       <c r="F8" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="H8" s="6">
+        <v>6</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="J8" s="27">
+        <v>44195</v>
+      </c>
+      <c r="L8" s="30">
+        <v>6</v>
+      </c>
+      <c r="M8" s="30">
+        <v>9</v>
+      </c>
+      <c r="N8" s="30">
+        <v>9</v>
+      </c>
+      <c r="O8" s="30">
+        <v>6</v>
+      </c>
+      <c r="P8" s="30">
+        <v>14</v>
+      </c>
+      <c r="Q8" s="30" t="s">
+        <v>281</v>
+      </c>
+      <c r="R8" s="30"/>
+      <c r="S8" s="30" t="s">
+        <v>283</v>
+      </c>
+      <c r="T8" s="31">
+        <v>44195</v>
+      </c>
+      <c r="U8" s="30" t="s">
+        <v>284</v>
+      </c>
+      <c r="V8" s="30"/>
+    </row>
+    <row r="9" spans="1:22" ht="34" x14ac:dyDescent="0.2">
       <c r="B9" s="1">
         <v>7</v>
       </c>
@@ -1477,8 +2001,46 @@
       <c r="F9" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="H9" s="6">
+        <v>7</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="J9" s="27">
+        <v>44195</v>
+      </c>
+      <c r="L9" s="30">
+        <v>7</v>
+      </c>
+      <c r="M9" s="30">
+        <v>2</v>
+      </c>
+      <c r="N9" s="30">
+        <v>10</v>
+      </c>
+      <c r="O9" s="30">
+        <v>19</v>
+      </c>
+      <c r="P9" s="30">
+        <v>10</v>
+      </c>
+      <c r="Q9" s="30" t="s">
+        <v>282</v>
+      </c>
+      <c r="R9" s="30"/>
+      <c r="S9" s="30" t="s">
+        <v>283</v>
+      </c>
+      <c r="T9" s="31">
+        <v>44203</v>
+      </c>
+      <c r="U9" s="30">
+        <v>0</v>
+      </c>
+      <c r="V9" s="30"/>
+    </row>
+    <row r="10" spans="1:22" ht="34" x14ac:dyDescent="0.2">
       <c r="B10" s="1">
         <v>8</v>
       </c>
@@ -1494,8 +2056,46 @@
       <c r="F10" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="H10" s="6">
+        <v>8</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="J10" s="27">
+        <v>44195</v>
+      </c>
+      <c r="L10" s="30">
+        <v>8</v>
+      </c>
+      <c r="M10" s="30">
+        <v>1</v>
+      </c>
+      <c r="N10" s="30">
+        <v>3</v>
+      </c>
+      <c r="O10" s="30">
+        <v>4</v>
+      </c>
+      <c r="P10" s="30">
+        <v>18</v>
+      </c>
+      <c r="Q10" s="30" t="s">
+        <v>310</v>
+      </c>
+      <c r="R10" s="30"/>
+      <c r="S10" s="30" t="s">
+        <v>283</v>
+      </c>
+      <c r="T10" s="31">
+        <v>44205</v>
+      </c>
+      <c r="U10" s="30">
+        <v>0</v>
+      </c>
+      <c r="V10" s="30"/>
+    </row>
+    <row r="11" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="B11" s="1">
         <v>9</v>
       </c>
@@ -1511,8 +2111,46 @@
       <c r="F11" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="H11" s="6">
+        <v>9</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="J11" s="27">
+        <v>44195</v>
+      </c>
+      <c r="L11" s="30">
+        <v>9</v>
+      </c>
+      <c r="M11" s="30">
+        <v>11</v>
+      </c>
+      <c r="N11" s="30">
+        <v>17</v>
+      </c>
+      <c r="O11" s="30">
+        <v>19</v>
+      </c>
+      <c r="P11" s="30">
+        <v>17</v>
+      </c>
+      <c r="Q11" s="30" t="s">
+        <v>312</v>
+      </c>
+      <c r="R11" s="30"/>
+      <c r="S11" s="34" t="s">
+        <v>283</v>
+      </c>
+      <c r="T11" s="31">
+        <v>44205</v>
+      </c>
+      <c r="U11" s="30">
+        <v>30</v>
+      </c>
+      <c r="V11" s="30"/>
+    </row>
+    <row r="12" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="B12" s="1">
         <v>10</v>
       </c>
@@ -1528,8 +2166,28 @@
       <c r="F12" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="13" spans="2:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="H12" s="6">
+        <v>10</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="J12" s="27">
+        <v>44203</v>
+      </c>
+      <c r="L12" s="30"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="30"/>
+      <c r="O12" s="30"/>
+      <c r="P12" s="30"/>
+      <c r="Q12" s="30"/>
+      <c r="R12" s="30"/>
+      <c r="S12" s="30"/>
+      <c r="T12" s="30"/>
+      <c r="U12" s="30"/>
+      <c r="V12" s="30"/>
+    </row>
+    <row r="13" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="B13" s="1">
         <v>11</v>
       </c>
@@ -1545,8 +2203,28 @@
       <c r="F13" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="2:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="H13" s="6">
+        <v>11</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="J13" s="27">
+        <v>44205</v>
+      </c>
+      <c r="L13" s="30"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="30"/>
+      <c r="O13" s="30"/>
+      <c r="P13" s="30"/>
+      <c r="Q13" s="30"/>
+      <c r="R13" s="30"/>
+      <c r="S13" s="30"/>
+      <c r="T13" s="30"/>
+      <c r="U13" s="30"/>
+      <c r="V13" s="30"/>
+    </row>
+    <row r="14" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="B14" s="1">
         <v>12</v>
       </c>
@@ -1562,8 +2240,22 @@
       <c r="F14" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="15" spans="2:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="30"/>
+      <c r="P14" s="30"/>
+      <c r="Q14" s="30"/>
+      <c r="R14" s="30"/>
+      <c r="S14" s="30"/>
+      <c r="T14" s="30"/>
+      <c r="U14" s="30"/>
+      <c r="V14" s="30"/>
+    </row>
+    <row r="15" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="B15" s="1">
         <v>13</v>
       </c>
@@ -1579,8 +2271,22 @@
       <c r="F15" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="16" spans="2:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="L15" s="30"/>
+      <c r="M15" s="30"/>
+      <c r="N15" s="30"/>
+      <c r="O15" s="30"/>
+      <c r="P15" s="30"/>
+      <c r="Q15" s="30"/>
+      <c r="R15" s="30"/>
+      <c r="S15" s="30"/>
+      <c r="T15" s="30"/>
+      <c r="U15" s="30"/>
+      <c r="V15" s="30"/>
+    </row>
+    <row r="16" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="B16" s="1">
         <v>14</v>
       </c>
@@ -1596,8 +2302,19 @@
       <c r="F16" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="2:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="L16" s="30"/>
+      <c r="M16" s="30"/>
+      <c r="N16" s="30"/>
+      <c r="O16" s="30"/>
+      <c r="P16" s="30"/>
+      <c r="Q16" s="30"/>
+      <c r="R16" s="30"/>
+      <c r="S16" s="30"/>
+      <c r="T16" s="30"/>
+      <c r="U16" s="30"/>
+      <c r="V16" s="30"/>
+    </row>
+    <row r="17" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="B17" s="1">
         <v>15</v>
       </c>
@@ -1614,7 +2331,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="2:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="B18" s="1">
         <v>16</v>
       </c>
@@ -1631,7 +2348,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="2:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="B19" s="1">
         <v>17</v>
       </c>
@@ -1647,8 +2364,9 @@
       <c r="F19" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="20" spans="2:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="O19" s="33"/>
+    </row>
+    <row r="20" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="B20" s="1">
         <v>18</v>
       </c>
@@ -1665,7 +2383,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="2:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="B21" s="1">
         <v>19</v>
       </c>
@@ -1682,7 +2400,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="2:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="B22" s="1">
         <v>20</v>
       </c>
@@ -1699,28 +2417,31 @@
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="2:14" ht="22" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18" ht="22" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>250</v>
+      </c>
       <c r="B26" s="4" t="s">
         <v>63</v>
       </c>
@@ -1758,8 +2479,20 @@
         <v>74</v>
       </c>
       <c r="N26" s="6"/>
-    </row>
-    <row r="27" spans="2:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="O26" s="32" t="s">
+        <v>285</v>
+      </c>
+      <c r="P26" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="Q26" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="R26" s="5" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="B27" s="8">
         <v>1</v>
       </c>
@@ -1795,8 +2528,17 @@
       </c>
       <c r="M27" s="8"/>
       <c r="N27" s="8"/>
-    </row>
-    <row r="28" spans="2:14" ht="19" x14ac:dyDescent="0.2">
+      <c r="P27" s="29">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="29" t="s">
+        <v>288</v>
+      </c>
+      <c r="R27" s="29" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="B28" s="8">
         <v>2</v>
       </c>
@@ -1832,8 +2574,17 @@
       </c>
       <c r="M28" s="8"/>
       <c r="N28" s="8"/>
-    </row>
-    <row r="29" spans="2:14" ht="19" x14ac:dyDescent="0.2">
+      <c r="P28" s="29">
+        <v>2</v>
+      </c>
+      <c r="Q28" s="29" t="s">
+        <v>289</v>
+      </c>
+      <c r="R28" s="29" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="B29" s="8">
         <v>3</v>
       </c>
@@ -1869,8 +2620,17 @@
       </c>
       <c r="M29" s="8"/>
       <c r="N29" s="8"/>
-    </row>
-    <row r="30" spans="2:14" ht="19" x14ac:dyDescent="0.2">
+      <c r="P29" s="29">
+        <v>3</v>
+      </c>
+      <c r="Q29" s="29" t="s">
+        <v>290</v>
+      </c>
+      <c r="R29" s="29" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="B30" s="8">
         <v>4</v>
       </c>
@@ -1906,8 +2666,17 @@
       </c>
       <c r="M30" s="8"/>
       <c r="N30" s="8"/>
-    </row>
-    <row r="31" spans="2:14" ht="19" x14ac:dyDescent="0.2">
+      <c r="P30" s="29">
+        <v>4</v>
+      </c>
+      <c r="Q30" s="29" t="s">
+        <v>291</v>
+      </c>
+      <c r="R30" s="29" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="B31" s="8">
         <v>5</v>
       </c>
@@ -1943,8 +2712,17 @@
       </c>
       <c r="M31" s="8"/>
       <c r="N31" s="8"/>
-    </row>
-    <row r="32" spans="2:14" ht="19" x14ac:dyDescent="0.2">
+      <c r="P31" s="29">
+        <v>5</v>
+      </c>
+      <c r="Q31" s="29" t="s">
+        <v>292</v>
+      </c>
+      <c r="R31" s="29" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" ht="19" x14ac:dyDescent="0.2">
       <c r="B32" s="8">
         <v>6</v>
       </c>
@@ -1980,8 +2758,17 @@
       </c>
       <c r="M32" s="8"/>
       <c r="N32" s="8"/>
-    </row>
-    <row r="33" spans="2:14" ht="19" x14ac:dyDescent="0.2">
+      <c r="P32" s="29">
+        <v>6</v>
+      </c>
+      <c r="Q32" s="29" t="s">
+        <v>293</v>
+      </c>
+      <c r="R32" s="29" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="33" spans="2:18" ht="19" x14ac:dyDescent="0.2">
       <c r="B33" s="8">
         <v>7</v>
       </c>
@@ -2017,8 +2804,17 @@
       </c>
       <c r="M33" s="8"/>
       <c r="N33" s="8"/>
-    </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="P33" s="29">
+        <v>7</v>
+      </c>
+      <c r="Q33" s="29" t="s">
+        <v>294</v>
+      </c>
+      <c r="R33" s="29" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="34" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B34" s="8">
         <v>8</v>
       </c>
@@ -2054,8 +2850,17 @@
       </c>
       <c r="M34" s="8"/>
       <c r="N34" s="8"/>
-    </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="P34" s="29">
+        <v>8</v>
+      </c>
+      <c r="Q34" s="29" t="s">
+        <v>295</v>
+      </c>
+      <c r="R34" s="29" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="35" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B35" s="8">
         <v>9</v>
       </c>
@@ -2093,8 +2898,17 @@
         <v>118</v>
       </c>
       <c r="N35" s="8"/>
-    </row>
-    <row r="36" spans="2:14" ht="19" x14ac:dyDescent="0.2">
+      <c r="P35" s="29">
+        <v>9</v>
+      </c>
+      <c r="Q35" s="29" t="s">
+        <v>278</v>
+      </c>
+      <c r="R35" s="29" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="36" spans="2:18" ht="19" x14ac:dyDescent="0.2">
       <c r="B36" s="8">
         <v>10</v>
       </c>
@@ -2130,8 +2944,17 @@
       </c>
       <c r="M36" s="8"/>
       <c r="N36" s="8"/>
-    </row>
-    <row r="37" spans="2:14" ht="19" x14ac:dyDescent="0.2">
+      <c r="P36" s="29">
+        <v>10</v>
+      </c>
+      <c r="Q36" s="29" t="s">
+        <v>296</v>
+      </c>
+      <c r="R36" s="29" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="37" spans="2:18" ht="19" x14ac:dyDescent="0.2">
       <c r="B37" s="8">
         <v>11</v>
       </c>
@@ -2167,8 +2990,17 @@
       </c>
       <c r="M37" s="8"/>
       <c r="N37" s="8"/>
-    </row>
-    <row r="38" spans="2:14" ht="19" x14ac:dyDescent="0.2">
+      <c r="P37" s="29">
+        <v>11</v>
+      </c>
+      <c r="Q37" s="29" t="s">
+        <v>297</v>
+      </c>
+      <c r="R37" s="29" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="38" spans="2:18" ht="19" x14ac:dyDescent="0.2">
       <c r="B38" s="8">
         <v>12</v>
       </c>
@@ -2204,8 +3036,17 @@
       </c>
       <c r="M38" s="8"/>
       <c r="N38" s="8"/>
-    </row>
-    <row r="39" spans="2:14" ht="19" x14ac:dyDescent="0.2">
+      <c r="P38" s="29">
+        <v>12</v>
+      </c>
+      <c r="Q38" s="29" t="s">
+        <v>298</v>
+      </c>
+      <c r="R38" s="29" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="39" spans="2:18" ht="19" x14ac:dyDescent="0.2">
       <c r="B39" s="8">
         <v>13</v>
       </c>
@@ -2241,8 +3082,17 @@
       </c>
       <c r="M39" s="8"/>
       <c r="N39" s="8"/>
-    </row>
-    <row r="40" spans="2:14" ht="19" x14ac:dyDescent="0.2">
+      <c r="P39" s="29">
+        <v>13</v>
+      </c>
+      <c r="Q39" s="29" t="s">
+        <v>299</v>
+      </c>
+      <c r="R39" s="29" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="40" spans="2:18" ht="19" x14ac:dyDescent="0.2">
       <c r="B40" s="8">
         <v>14</v>
       </c>
@@ -2278,8 +3128,17 @@
       </c>
       <c r="M40" s="8"/>
       <c r="N40" s="8"/>
-    </row>
-    <row r="41" spans="2:14" ht="19" x14ac:dyDescent="0.2">
+      <c r="P40" s="29">
+        <v>14</v>
+      </c>
+      <c r="Q40" s="29" t="s">
+        <v>300</v>
+      </c>
+      <c r="R40" s="29" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="41" spans="2:18" ht="19" x14ac:dyDescent="0.2">
       <c r="B41" s="8">
         <v>15</v>
       </c>
@@ -2315,8 +3174,15 @@
       </c>
       <c r="M41" s="8"/>
       <c r="N41" s="8"/>
-    </row>
-    <row r="42" spans="2:14" ht="19" x14ac:dyDescent="0.2">
+      <c r="P41" s="29">
+        <v>15</v>
+      </c>
+      <c r="Q41" s="29"/>
+      <c r="R41" s="29" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="42" spans="2:18" ht="19" x14ac:dyDescent="0.2">
       <c r="B42" s="8">
         <v>16</v>
       </c>
@@ -2352,8 +3218,17 @@
       </c>
       <c r="M42" s="8"/>
       <c r="N42" s="8"/>
-    </row>
-    <row r="43" spans="2:14" ht="19" x14ac:dyDescent="0.2">
+      <c r="P42" s="29">
+        <v>16</v>
+      </c>
+      <c r="Q42" s="29" t="s">
+        <v>314</v>
+      </c>
+      <c r="R42" s="29" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="43" spans="2:18" ht="19" x14ac:dyDescent="0.2">
       <c r="B43" s="11">
         <v>17</v>
       </c>
@@ -2391,8 +3266,17 @@
         <v>166</v>
       </c>
       <c r="N43" s="8"/>
-    </row>
-    <row r="44" spans="2:14" ht="19" x14ac:dyDescent="0.2">
+      <c r="P43" s="29">
+        <v>17</v>
+      </c>
+      <c r="Q43" s="29" t="s">
+        <v>313</v>
+      </c>
+      <c r="R43" s="29" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="44" spans="2:18" ht="19" x14ac:dyDescent="0.2">
       <c r="B44" s="11">
         <v>18</v>
       </c>
@@ -2428,8 +3312,15 @@
       </c>
       <c r="M44" s="8"/>
       <c r="N44" s="8"/>
-    </row>
-    <row r="45" spans="2:14" ht="19" x14ac:dyDescent="0.2">
+      <c r="P44" s="29">
+        <v>18</v>
+      </c>
+      <c r="Q44" s="29"/>
+      <c r="R44" s="29" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="45" spans="2:18" ht="19" x14ac:dyDescent="0.2">
       <c r="B45" s="11">
         <v>19</v>
       </c>
@@ -2465,8 +3356,11 @@
       </c>
       <c r="M45" s="8"/>
       <c r="N45" s="8"/>
-    </row>
-    <row r="46" spans="2:14" ht="19" x14ac:dyDescent="0.2">
+      <c r="P45" s="29"/>
+      <c r="Q45" s="29"/>
+      <c r="R45" s="29"/>
+    </row>
+    <row r="46" spans="2:18" ht="19" x14ac:dyDescent="0.2">
       <c r="B46" s="11">
         <v>20</v>
       </c>
@@ -2502,6 +3396,9 @@
       </c>
       <c r="M46" s="8"/>
       <c r="N46" s="8"/>
+      <c r="P46" s="29"/>
+      <c r="Q46" s="29"/>
+      <c r="R46" s="29"/>
     </row>
     <row r="50" spans="2:6" ht="21" x14ac:dyDescent="0.25">
       <c r="B50" s="15" t="s">
@@ -2526,13 +3423,13 @@
       </c>
     </row>
     <row r="53" spans="2:6" ht="36" x14ac:dyDescent="0.25">
-      <c r="B53" s="18" t="s">
+      <c r="B53" s="22" t="s">
         <v>220</v>
       </c>
       <c r="C53" s="17" t="s">
         <v>221</v>
       </c>
-      <c r="D53" s="23" t="s">
+      <c r="D53" s="20" t="s">
         <v>227</v>
       </c>
       <c r="E53" s="17"/>
@@ -2541,11 +3438,11 @@
       </c>
     </row>
     <row r="54" spans="2:6" ht="54" x14ac:dyDescent="0.25">
-      <c r="B54" s="19"/>
+      <c r="B54" s="23"/>
       <c r="C54" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="D54" s="23" t="s">
+      <c r="D54" s="20" t="s">
         <v>224</v>
       </c>
       <c r="E54" s="17"/>
@@ -2554,11 +3451,11 @@
       </c>
     </row>
     <row r="55" spans="2:6" ht="72" x14ac:dyDescent="0.25">
-      <c r="B55" s="19"/>
+      <c r="B55" s="23"/>
       <c r="C55" s="17" t="s">
         <v>231</v>
       </c>
-      <c r="D55" s="23" t="s">
+      <c r="D55" s="20" t="s">
         <v>225</v>
       </c>
       <c r="E55" s="17"/>
@@ -2567,11 +3464,11 @@
       </c>
     </row>
     <row r="56" spans="2:6" ht="54" x14ac:dyDescent="0.25">
-      <c r="B56" s="19"/>
+      <c r="B56" s="23"/>
       <c r="C56" s="17" t="s">
         <v>226</v>
       </c>
-      <c r="D56" s="23" t="s">
+      <c r="D56" s="20" t="s">
         <v>228</v>
       </c>
       <c r="E56" s="17"/>
@@ -2580,11 +3477,11 @@
       </c>
     </row>
     <row r="57" spans="2:6" ht="54" x14ac:dyDescent="0.25">
-      <c r="B57" s="19"/>
+      <c r="B57" s="23"/>
       <c r="C57" s="17" t="s">
         <v>232</v>
       </c>
-      <c r="D57" s="24" t="s">
+      <c r="D57" s="21" t="s">
         <v>234</v>
       </c>
       <c r="E57" s="17"/>
@@ -2593,11 +3490,11 @@
       </c>
     </row>
     <row r="58" spans="2:6" ht="54" x14ac:dyDescent="0.25">
-      <c r="B58" s="19"/>
-      <c r="C58" s="22" t="s">
+      <c r="B58" s="23"/>
+      <c r="C58" s="19" t="s">
         <v>235</v>
       </c>
-      <c r="D58" s="23" t="s">
+      <c r="D58" s="20" t="s">
         <v>236</v>
       </c>
       <c r="E58" s="17"/>
@@ -2606,11 +3503,11 @@
       </c>
     </row>
     <row r="59" spans="2:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="B59" s="19"/>
+      <c r="B59" s="23"/>
       <c r="C59" s="17" t="s">
         <v>237</v>
       </c>
-      <c r="D59" s="23" t="s">
+      <c r="D59" s="20" t="s">
         <v>238</v>
       </c>
       <c r="E59" s="17" t="s">
@@ -2621,11 +3518,11 @@
       </c>
     </row>
     <row r="60" spans="2:6" ht="72" x14ac:dyDescent="0.25">
-      <c r="B60" s="19"/>
+      <c r="B60" s="23"/>
       <c r="C60" s="17" t="s">
         <v>240</v>
       </c>
-      <c r="D60" s="23" t="s">
+      <c r="D60" s="20" t="s">
         <v>241</v>
       </c>
       <c r="E60" s="17"/>
@@ -2634,20 +3531,20 @@
       </c>
     </row>
     <row r="61" spans="2:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="B61" s="20"/>
+      <c r="B61" s="24"/>
       <c r="C61" s="17"/>
-      <c r="D61" s="23"/>
+      <c r="D61" s="20"/>
       <c r="E61" s="17"/>
       <c r="F61" s="17"/>
     </row>
     <row r="62" spans="2:6" ht="54" x14ac:dyDescent="0.25">
-      <c r="B62" s="18" t="s">
+      <c r="B62" s="22" t="s">
         <v>242</v>
       </c>
       <c r="C62" s="17" t="s">
         <v>244</v>
       </c>
-      <c r="D62" s="23" t="s">
+      <c r="D62" s="20" t="s">
         <v>245</v>
       </c>
       <c r="E62" s="17"/>
@@ -2656,11 +3553,11 @@
       </c>
     </row>
     <row r="63" spans="2:6" ht="120" x14ac:dyDescent="0.25">
-      <c r="B63" s="19"/>
+      <c r="B63" s="23"/>
       <c r="C63" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="D63" s="23" t="s">
+      <c r="D63" s="20" t="s">
         <v>247</v>
       </c>
       <c r="E63" s="17" t="s">
@@ -2671,130 +3568,130 @@
       </c>
     </row>
     <row r="64" spans="2:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="B64" s="19"/>
+      <c r="B64" s="23"/>
       <c r="C64" s="17"/>
-      <c r="D64" s="23"/>
+      <c r="D64" s="20"/>
       <c r="E64" s="17"/>
       <c r="F64" s="17"/>
     </row>
     <row r="65" spans="2:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="B65" s="19"/>
+      <c r="B65" s="23"/>
       <c r="C65" s="17"/>
-      <c r="D65" s="23"/>
+      <c r="D65" s="20"/>
       <c r="E65" s="17"/>
       <c r="F65" s="17"/>
     </row>
     <row r="66" spans="2:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="B66" s="19"/>
+      <c r="B66" s="23"/>
       <c r="C66" s="17"/>
-      <c r="D66" s="23"/>
+      <c r="D66" s="20"/>
       <c r="E66" s="17"/>
       <c r="F66" s="17"/>
     </row>
     <row r="67" spans="2:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="B67" s="19"/>
+      <c r="B67" s="23"/>
       <c r="C67" s="17"/>
-      <c r="D67" s="23"/>
+      <c r="D67" s="20"/>
       <c r="E67" s="17"/>
       <c r="F67" s="17"/>
     </row>
     <row r="68" spans="2:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="B68" s="19"/>
+      <c r="B68" s="23"/>
       <c r="C68" s="17"/>
-      <c r="D68" s="23"/>
+      <c r="D68" s="20"/>
       <c r="E68" s="17"/>
       <c r="F68" s="17"/>
     </row>
     <row r="69" spans="2:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="B69" s="20"/>
+      <c r="B69" s="24"/>
       <c r="C69" s="17"/>
-      <c r="D69" s="23"/>
+      <c r="D69" s="20"/>
       <c r="E69" s="17"/>
       <c r="F69" s="17"/>
     </row>
     <row r="70" spans="2:6" ht="17" x14ac:dyDescent="0.25">
       <c r="B70" s="17"/>
       <c r="C70" s="17"/>
-      <c r="D70" s="23"/>
+      <c r="D70" s="20"/>
       <c r="E70" s="17"/>
       <c r="F70" s="17"/>
     </row>
     <row r="71" spans="2:6" ht="17" x14ac:dyDescent="0.25">
       <c r="B71" s="17"/>
       <c r="C71" s="17"/>
-      <c r="D71" s="23"/>
+      <c r="D71" s="20"/>
       <c r="E71" s="17"/>
       <c r="F71" s="17"/>
     </row>
     <row r="72" spans="2:6" ht="17" x14ac:dyDescent="0.25">
       <c r="B72" s="17"/>
       <c r="C72" s="17"/>
-      <c r="D72" s="23"/>
+      <c r="D72" s="20"/>
       <c r="E72" s="17"/>
       <c r="F72" s="17"/>
     </row>
     <row r="73" spans="2:6" ht="17" x14ac:dyDescent="0.25">
       <c r="B73" s="17"/>
       <c r="C73" s="17"/>
-      <c r="D73" s="23"/>
+      <c r="D73" s="20"/>
       <c r="E73" s="17"/>
       <c r="F73" s="17"/>
     </row>
     <row r="74" spans="2:6" ht="17" x14ac:dyDescent="0.25">
       <c r="B74" s="17"/>
       <c r="C74" s="17"/>
-      <c r="D74" s="23"/>
+      <c r="D74" s="20"/>
       <c r="E74" s="17"/>
       <c r="F74" s="17"/>
     </row>
     <row r="75" spans="2:6" ht="17" x14ac:dyDescent="0.25">
       <c r="B75" s="17"/>
       <c r="C75" s="17"/>
-      <c r="D75" s="23"/>
+      <c r="D75" s="20"/>
       <c r="E75" s="17"/>
       <c r="F75" s="17"/>
     </row>
     <row r="76" spans="2:6" ht="17" x14ac:dyDescent="0.25">
       <c r="B76" s="17"/>
       <c r="C76" s="17"/>
-      <c r="D76" s="23"/>
+      <c r="D76" s="20"/>
       <c r="E76" s="17"/>
       <c r="F76" s="17"/>
     </row>
     <row r="77" spans="2:6" ht="17" x14ac:dyDescent="0.25">
       <c r="B77" s="17"/>
       <c r="C77" s="17"/>
-      <c r="D77" s="23"/>
+      <c r="D77" s="20"/>
       <c r="E77" s="17"/>
       <c r="F77" s="17"/>
     </row>
     <row r="78" spans="2:6" ht="17" x14ac:dyDescent="0.25">
       <c r="B78" s="17"/>
       <c r="C78" s="17"/>
-      <c r="D78" s="23"/>
+      <c r="D78" s="20"/>
       <c r="E78" s="17"/>
       <c r="F78" s="17"/>
     </row>
     <row r="79" spans="2:6" ht="17" x14ac:dyDescent="0.25">
       <c r="B79" s="17"/>
       <c r="C79" s="17"/>
-      <c r="D79" s="23"/>
+      <c r="D79" s="20"/>
       <c r="E79" s="17"/>
       <c r="F79" s="17"/>
     </row>
     <row r="80" spans="2:6" ht="17" x14ac:dyDescent="0.25">
       <c r="B80" s="17"/>
       <c r="C80" s="17"/>
-      <c r="D80" s="23"/>
+      <c r="D80" s="20"/>
       <c r="E80" s="17"/>
       <c r="F80" s="17"/>
     </row>
     <row r="81" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B81" s="21"/>
-      <c r="C81" s="21"/>
-      <c r="D81" s="21"/>
-      <c r="E81" s="21"/>
-      <c r="F81" s="21"/>
+      <c r="B81" s="18"/>
+      <c r="C81" s="18"/>
+      <c r="D81" s="18"/>
+      <c r="E81" s="18"/>
+      <c r="F81" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
ajout de nouvelles données à la base et ecriture de nouvelles requêtes de tests
</commit_message>
<xml_diff>
--- a/bdd/infos_bdd.xlsx
+++ b/bdd/infos_bdd.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marieeonnet/Documents/Documents - MacBook Pro de Marie/Cours_DUT_Caen/Projet2A/dut2021_pret_instruments_voyage/bdd/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB53432-AE3F-7841-B70E-557690525DE7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC1A2DDC-2973-F348-82A5-CB603AEA53B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="500" windowWidth="24380" windowHeight="17020" xr2:uid="{1C6F6E9A-B456-E643-B447-123029CC3B3E}"/>
+    <workbookView xWindow="32700" yWindow="1020" windowWidth="33040" windowHeight="17660" xr2:uid="{1C6F6E9A-B456-E643-B447-123029CC3B3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="322">
   <si>
     <t>Vil_nom</t>
   </si>
@@ -979,6 +979,27 @@
   </si>
   <si>
     <t>Piano</t>
+  </si>
+  <si>
+    <t>Shiver</t>
+  </si>
+  <si>
+    <t>Maracs</t>
+  </si>
+  <si>
+    <t>Fender Straocaster</t>
+  </si>
+  <si>
+    <t>Violon Silencieux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oui </t>
+  </si>
+  <si>
+    <t>Stentor</t>
+  </si>
+  <si>
+    <t>Gliga</t>
   </si>
 </sst>
 </file>
@@ -1141,7 +1162,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1204,15 +1225,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1243,6 +1255,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1560,8 +1585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D70755CD-10D4-DA48-863B-E92693C8657B}">
   <dimension ref="A2:V81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M4" workbookViewId="0">
-      <selection activeCell="U27" sqref="U27"/>
+    <sheetView tabSelected="1" topLeftCell="F12" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1606,52 +1631,52 @@
       <c r="F2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="22" t="s">
         <v>251</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="H2" s="23" t="s">
         <v>252</v>
       </c>
-      <c r="I2" s="26" t="s">
+      <c r="I2" s="23" t="s">
         <v>253</v>
       </c>
-      <c r="J2" s="26" t="s">
+      <c r="J2" s="23" t="s">
         <v>254</v>
       </c>
-      <c r="K2" s="28" t="s">
+      <c r="K2" s="25" t="s">
         <v>265</v>
       </c>
-      <c r="L2" s="26" t="s">
+      <c r="L2" s="23" t="s">
         <v>266</v>
       </c>
-      <c r="M2" s="26" t="s">
+      <c r="M2" s="23" t="s">
         <v>252</v>
       </c>
-      <c r="N2" s="26" t="s">
+      <c r="N2" s="23" t="s">
         <v>267</v>
       </c>
-      <c r="O2" s="26" t="s">
+      <c r="O2" s="23" t="s">
         <v>268</v>
       </c>
-      <c r="P2" s="26" t="s">
+      <c r="P2" s="23" t="s">
         <v>269</v>
       </c>
-      <c r="Q2" s="26" t="s">
+      <c r="Q2" s="23" t="s">
         <v>270</v>
       </c>
-      <c r="R2" s="26" t="s">
+      <c r="R2" s="23" t="s">
         <v>271</v>
       </c>
-      <c r="S2" s="26" t="s">
+      <c r="S2" s="23" t="s">
         <v>272</v>
       </c>
-      <c r="T2" s="26" t="s">
+      <c r="T2" s="23" t="s">
         <v>273</v>
       </c>
-      <c r="U2" s="26" t="s">
+      <c r="U2" s="23" t="s">
         <v>274</v>
       </c>
-      <c r="V2" s="26" t="s">
+      <c r="V2" s="23" t="s">
         <v>275</v>
       </c>
     </row>
@@ -1677,38 +1702,38 @@
       <c r="I3" s="6" t="s">
         <v>255</v>
       </c>
-      <c r="J3" s="27">
+      <c r="J3" s="24">
         <v>44195</v>
       </c>
-      <c r="L3" s="30">
+      <c r="L3" s="27">
         <v>1</v>
       </c>
-      <c r="M3" s="30">
+      <c r="M3" s="27">
         <v>1</v>
       </c>
-      <c r="N3" s="30">
+      <c r="N3" s="27">
         <v>1</v>
       </c>
-      <c r="O3" s="30">
+      <c r="O3" s="27">
         <v>1</v>
       </c>
-      <c r="P3" s="30">
+      <c r="P3" s="27">
         <v>2</v>
       </c>
-      <c r="Q3" s="30" t="s">
+      <c r="Q3" s="27" t="s">
         <v>276</v>
       </c>
-      <c r="R3" s="30"/>
-      <c r="S3" s="30" t="s">
+      <c r="R3" s="27"/>
+      <c r="S3" s="27" t="s">
         <v>283</v>
       </c>
-      <c r="T3" s="31">
+      <c r="T3" s="28">
         <v>44203</v>
       </c>
-      <c r="U3" s="30">
+      <c r="U3" s="27">
         <v>0</v>
       </c>
-      <c r="V3" s="30"/>
+      <c r="V3" s="27"/>
     </row>
     <row r="4" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="B4" s="1">
@@ -1732,38 +1757,38 @@
       <c r="I4" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="J4" s="27">
+      <c r="J4" s="24">
         <v>44195</v>
       </c>
-      <c r="L4" s="30">
+      <c r="L4" s="27">
         <v>2</v>
       </c>
-      <c r="M4" s="30">
+      <c r="M4" s="27">
         <v>4</v>
       </c>
-      <c r="N4" s="30">
+      <c r="N4" s="27">
         <v>4</v>
       </c>
-      <c r="O4" s="30">
+      <c r="O4" s="27">
         <v>4</v>
       </c>
-      <c r="P4" s="30">
+      <c r="P4" s="27">
         <v>1</v>
       </c>
-      <c r="Q4" s="30" t="s">
+      <c r="Q4" s="27" t="s">
         <v>277</v>
       </c>
-      <c r="R4" s="30"/>
-      <c r="S4" s="30" t="s">
+      <c r="R4" s="27"/>
+      <c r="S4" s="27" t="s">
         <v>283</v>
       </c>
-      <c r="T4" s="31">
+      <c r="T4" s="28">
         <v>44195</v>
       </c>
-      <c r="U4" s="30">
+      <c r="U4" s="27">
         <v>99</v>
       </c>
-      <c r="V4" s="30"/>
+      <c r="V4" s="27"/>
     </row>
     <row r="5" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="B5" s="1">
@@ -1787,38 +1812,38 @@
       <c r="I5" s="6" t="s">
         <v>257</v>
       </c>
-      <c r="J5" s="27">
+      <c r="J5" s="24">
         <v>44195</v>
       </c>
-      <c r="L5" s="30">
+      <c r="L5" s="27">
         <v>3</v>
       </c>
-      <c r="M5" s="30">
+      <c r="M5" s="27">
         <v>2</v>
       </c>
-      <c r="N5" s="30">
+      <c r="N5" s="27">
         <v>18</v>
       </c>
-      <c r="O5" s="30">
+      <c r="O5" s="27">
         <v>15</v>
       </c>
-      <c r="P5" s="30">
+      <c r="P5" s="27">
         <v>9</v>
       </c>
-      <c r="Q5" s="30" t="s">
+      <c r="Q5" s="27" t="s">
         <v>278</v>
       </c>
-      <c r="R5" s="30"/>
-      <c r="S5" s="30" t="s">
+      <c r="R5" s="27"/>
+      <c r="S5" s="27" t="s">
         <v>283</v>
       </c>
-      <c r="T5" s="31">
+      <c r="T5" s="28">
         <v>44203</v>
       </c>
-      <c r="U5" s="30">
-        <v>0</v>
-      </c>
-      <c r="V5" s="30"/>
+      <c r="U5" s="27">
+        <v>10</v>
+      </c>
+      <c r="V5" s="27"/>
     </row>
     <row r="6" spans="1:22" ht="34" x14ac:dyDescent="0.2">
       <c r="B6" s="1">
@@ -1842,38 +1867,38 @@
       <c r="I6" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="J6" s="27">
+      <c r="J6" s="24">
         <v>44195</v>
       </c>
-      <c r="L6" s="30">
+      <c r="L6" s="27">
         <v>4</v>
       </c>
-      <c r="M6" s="30">
+      <c r="M6" s="27">
         <v>6</v>
       </c>
-      <c r="N6" s="30">
+      <c r="N6" s="27">
         <v>13</v>
       </c>
-      <c r="O6" s="30">
+      <c r="O6" s="27">
         <v>18</v>
       </c>
-      <c r="P6" s="30">
+      <c r="P6" s="27">
         <v>11</v>
       </c>
-      <c r="Q6" s="30" t="s">
+      <c r="Q6" s="27" t="s">
         <v>279</v>
       </c>
-      <c r="R6" s="30"/>
-      <c r="S6" s="30" t="s">
+      <c r="R6" s="27"/>
+      <c r="S6" s="27" t="s">
         <v>283</v>
       </c>
-      <c r="T6" s="31">
+      <c r="T6" s="28">
         <v>44195</v>
       </c>
-      <c r="U6" s="30">
-        <v>10</v>
-      </c>
-      <c r="V6" s="30"/>
+      <c r="U6" s="27">
+        <v>0</v>
+      </c>
+      <c r="V6" s="27"/>
     </row>
     <row r="7" spans="1:22" ht="34" x14ac:dyDescent="0.2">
       <c r="B7" s="1">
@@ -1897,38 +1922,38 @@
       <c r="I7" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="J7" s="27">
+      <c r="J7" s="24">
         <v>44195</v>
       </c>
-      <c r="L7" s="30">
+      <c r="L7" s="27">
         <v>5</v>
       </c>
-      <c r="M7" s="30">
+      <c r="M7" s="27">
         <v>10</v>
       </c>
-      <c r="N7" s="30">
+      <c r="N7" s="27">
         <v>19</v>
       </c>
-      <c r="O7" s="30">
+      <c r="O7" s="27">
         <v>22</v>
       </c>
-      <c r="P7" s="30">
+      <c r="P7" s="27">
         <v>13</v>
       </c>
-      <c r="Q7" s="30" t="s">
+      <c r="Q7" s="27" t="s">
         <v>280</v>
       </c>
-      <c r="R7" s="30"/>
-      <c r="S7" s="30" t="s">
+      <c r="R7" s="27"/>
+      <c r="S7" s="27" t="s">
         <v>283</v>
       </c>
-      <c r="T7" s="31">
+      <c r="T7" s="28">
         <v>44203</v>
       </c>
-      <c r="U7" s="30">
+      <c r="U7" s="27">
         <v>0</v>
       </c>
-      <c r="V7" s="30"/>
+      <c r="V7" s="27"/>
     </row>
     <row r="8" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" s="1">
@@ -1952,38 +1977,38 @@
       <c r="I8" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="J8" s="27">
+      <c r="J8" s="24">
         <v>44195</v>
       </c>
-      <c r="L8" s="30">
+      <c r="L8" s="27">
         <v>6</v>
       </c>
-      <c r="M8" s="30">
+      <c r="M8" s="27">
         <v>9</v>
       </c>
-      <c r="N8" s="30">
+      <c r="N8" s="27">
         <v>9</v>
       </c>
-      <c r="O8" s="30">
+      <c r="O8" s="27">
         <v>6</v>
       </c>
-      <c r="P8" s="30">
+      <c r="P8" s="27">
         <v>14</v>
       </c>
-      <c r="Q8" s="30" t="s">
+      <c r="Q8" s="27" t="s">
         <v>281</v>
       </c>
-      <c r="R8" s="30"/>
-      <c r="S8" s="30" t="s">
+      <c r="R8" s="27"/>
+      <c r="S8" s="27" t="s">
         <v>283</v>
       </c>
-      <c r="T8" s="31">
+      <c r="T8" s="28">
         <v>44195</v>
       </c>
-      <c r="U8" s="30" t="s">
+      <c r="U8" s="27" t="s">
         <v>284</v>
       </c>
-      <c r="V8" s="30"/>
+      <c r="V8" s="27"/>
     </row>
     <row r="9" spans="1:22" ht="34" x14ac:dyDescent="0.2">
       <c r="B9" s="1">
@@ -2007,38 +2032,38 @@
       <c r="I9" s="6" t="s">
         <v>261</v>
       </c>
-      <c r="J9" s="27">
+      <c r="J9" s="24">
         <v>44195</v>
       </c>
-      <c r="L9" s="30">
+      <c r="L9" s="27">
         <v>7</v>
       </c>
-      <c r="M9" s="30">
+      <c r="M9" s="27">
         <v>2</v>
       </c>
-      <c r="N9" s="30">
+      <c r="N9" s="27">
         <v>10</v>
       </c>
-      <c r="O9" s="30">
+      <c r="O9" s="27">
         <v>19</v>
       </c>
-      <c r="P9" s="30">
+      <c r="P9" s="27">
         <v>10</v>
       </c>
-      <c r="Q9" s="30" t="s">
+      <c r="Q9" s="27" t="s">
         <v>282</v>
       </c>
-      <c r="R9" s="30"/>
-      <c r="S9" s="30" t="s">
+      <c r="R9" s="27"/>
+      <c r="S9" s="27" t="s">
         <v>283</v>
       </c>
-      <c r="T9" s="31">
+      <c r="T9" s="28">
         <v>44203</v>
       </c>
-      <c r="U9" s="30">
+      <c r="U9" s="27">
         <v>0</v>
       </c>
-      <c r="V9" s="30"/>
+      <c r="V9" s="27"/>
     </row>
     <row r="10" spans="1:22" ht="34" x14ac:dyDescent="0.2">
       <c r="B10" s="1">
@@ -2062,38 +2087,38 @@
       <c r="I10" s="6" t="s">
         <v>262</v>
       </c>
-      <c r="J10" s="27">
+      <c r="J10" s="24">
         <v>44195</v>
       </c>
-      <c r="L10" s="30">
+      <c r="L10" s="27">
         <v>8</v>
       </c>
-      <c r="M10" s="30">
+      <c r="M10" s="27">
         <v>1</v>
       </c>
-      <c r="N10" s="30">
+      <c r="N10" s="27">
         <v>3</v>
       </c>
-      <c r="O10" s="30">
+      <c r="O10" s="27">
         <v>4</v>
       </c>
-      <c r="P10" s="30">
+      <c r="P10" s="27">
         <v>18</v>
       </c>
-      <c r="Q10" s="30" t="s">
+      <c r="Q10" s="27" t="s">
         <v>310</v>
       </c>
-      <c r="R10" s="30"/>
-      <c r="S10" s="30" t="s">
+      <c r="R10" s="27"/>
+      <c r="S10" s="27" t="s">
         <v>283</v>
       </c>
-      <c r="T10" s="31">
+      <c r="T10" s="28">
         <v>44205</v>
       </c>
-      <c r="U10" s="30">
+      <c r="U10" s="27">
         <v>0</v>
       </c>
-      <c r="V10" s="30"/>
+      <c r="V10" s="27"/>
     </row>
     <row r="11" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="B11" s="1">
@@ -2117,38 +2142,38 @@
       <c r="I11" s="6" t="s">
         <v>263</v>
       </c>
-      <c r="J11" s="27">
+      <c r="J11" s="24">
         <v>44195</v>
       </c>
-      <c r="L11" s="30">
+      <c r="L11" s="27">
         <v>9</v>
       </c>
-      <c r="M11" s="30">
+      <c r="M11" s="27">
         <v>11</v>
       </c>
-      <c r="N11" s="30">
+      <c r="N11" s="27">
         <v>17</v>
       </c>
-      <c r="O11" s="30">
+      <c r="O11" s="27">
         <v>19</v>
       </c>
-      <c r="P11" s="30">
+      <c r="P11" s="27">
         <v>17</v>
       </c>
-      <c r="Q11" s="30" t="s">
+      <c r="Q11" s="27" t="s">
         <v>312</v>
       </c>
-      <c r="R11" s="30"/>
-      <c r="S11" s="34" t="s">
+      <c r="R11" s="27"/>
+      <c r="S11" s="31" t="s">
         <v>283</v>
       </c>
-      <c r="T11" s="31">
+      <c r="T11" s="28">
         <v>44205</v>
       </c>
-      <c r="U11" s="30">
+      <c r="U11" s="27">
         <v>30</v>
       </c>
-      <c r="V11" s="30"/>
+      <c r="V11" s="27"/>
     </row>
     <row r="12" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="B12" s="1">
@@ -2172,20 +2197,38 @@
       <c r="I12" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="J12" s="27">
+      <c r="J12" s="24">
         <v>44203</v>
       </c>
-      <c r="L12" s="30"/>
-      <c r="M12" s="30"/>
-      <c r="N12" s="30"/>
-      <c r="O12" s="30"/>
-      <c r="P12" s="30"/>
-      <c r="Q12" s="30"/>
-      <c r="R12" s="30"/>
-      <c r="S12" s="30"/>
-      <c r="T12" s="30"/>
-      <c r="U12" s="30"/>
-      <c r="V12" s="30"/>
+      <c r="L12" s="27">
+        <v>10</v>
+      </c>
+      <c r="M12" s="27">
+        <v>12</v>
+      </c>
+      <c r="N12" s="27">
+        <v>11</v>
+      </c>
+      <c r="O12" s="27">
+        <v>17</v>
+      </c>
+      <c r="P12" s="27">
+        <v>4</v>
+      </c>
+      <c r="Q12" s="27" t="s">
+        <v>316</v>
+      </c>
+      <c r="R12" s="27"/>
+      <c r="S12" s="27" t="s">
+        <v>283</v>
+      </c>
+      <c r="T12" s="28">
+        <v>44206</v>
+      </c>
+      <c r="U12" s="27">
+        <v>0</v>
+      </c>
+      <c r="V12" s="27"/>
     </row>
     <row r="13" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="B13" s="1">
@@ -2209,20 +2252,38 @@
       <c r="I13" s="6" t="s">
         <v>311</v>
       </c>
-      <c r="J13" s="27">
+      <c r="J13" s="24">
         <v>44205</v>
       </c>
-      <c r="L13" s="30"/>
-      <c r="M13" s="30"/>
-      <c r="N13" s="30"/>
-      <c r="O13" s="30"/>
-      <c r="P13" s="30"/>
-      <c r="Q13" s="30"/>
-      <c r="R13" s="30"/>
-      <c r="S13" s="30"/>
-      <c r="T13" s="30"/>
-      <c r="U13" s="30"/>
-      <c r="V13" s="30"/>
+      <c r="L13" s="27">
+        <v>11</v>
+      </c>
+      <c r="M13" s="27">
+        <v>6</v>
+      </c>
+      <c r="N13" s="27">
+        <v>20</v>
+      </c>
+      <c r="O13" s="27">
+        <v>2</v>
+      </c>
+      <c r="P13" s="27">
+        <v>11</v>
+      </c>
+      <c r="Q13" s="27" t="s">
+        <v>317</v>
+      </c>
+      <c r="R13" s="27"/>
+      <c r="S13" s="27" t="s">
+        <v>283</v>
+      </c>
+      <c r="T13" s="28">
+        <v>44206</v>
+      </c>
+      <c r="U13" s="27">
+        <v>55</v>
+      </c>
+      <c r="V13" s="27"/>
     </row>
     <row r="14" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="B14" s="1">
@@ -2240,20 +2301,44 @@
       <c r="F14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="L14" s="30"/>
-      <c r="M14" s="30"/>
-      <c r="N14" s="30"/>
-      <c r="O14" s="30"/>
-      <c r="P14" s="30"/>
-      <c r="Q14" s="30"/>
-      <c r="R14" s="30"/>
-      <c r="S14" s="30"/>
-      <c r="T14" s="30"/>
-      <c r="U14" s="30"/>
-      <c r="V14" s="30"/>
+      <c r="H14" s="6">
+        <v>12</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="J14" s="24">
+        <v>44206</v>
+      </c>
+      <c r="L14" s="27">
+        <v>12</v>
+      </c>
+      <c r="M14" s="27">
+        <v>2</v>
+      </c>
+      <c r="N14" s="27">
+        <v>2</v>
+      </c>
+      <c r="O14" s="27">
+        <v>3</v>
+      </c>
+      <c r="P14" s="27">
+        <v>15</v>
+      </c>
+      <c r="Q14" s="27" t="s">
+        <v>318</v>
+      </c>
+      <c r="R14" s="27"/>
+      <c r="S14" s="27" t="s">
+        <v>319</v>
+      </c>
+      <c r="T14" s="28">
+        <v>44206</v>
+      </c>
+      <c r="U14" s="27">
+        <v>50</v>
+      </c>
+      <c r="V14" s="27"/>
     </row>
     <row r="15" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="B15" s="1">
@@ -2271,20 +2356,28 @@
       <c r="F15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="L15" s="30"/>
-      <c r="M15" s="30"/>
-      <c r="N15" s="30"/>
-      <c r="O15" s="30"/>
-      <c r="P15" s="30"/>
-      <c r="Q15" s="30"/>
-      <c r="R15" s="30"/>
-      <c r="S15" s="30"/>
-      <c r="T15" s="30"/>
-      <c r="U15" s="30"/>
-      <c r="V15" s="30"/>
+      <c r="H15" s="6">
+        <v>13</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="J15" s="24">
+        <v>44206</v>
+      </c>
+      <c r="L15" s="27">
+        <v>13</v>
+      </c>
+      <c r="M15" s="27"/>
+      <c r="N15" s="27"/>
+      <c r="O15" s="27"/>
+      <c r="P15" s="27"/>
+      <c r="Q15" s="27"/>
+      <c r="R15" s="27"/>
+      <c r="S15" s="27"/>
+      <c r="T15" s="27"/>
+      <c r="U15" s="27"/>
+      <c r="V15" s="27"/>
     </row>
     <row r="16" spans="1:22" ht="17" x14ac:dyDescent="0.2">
       <c r="B16" s="1">
@@ -2302,17 +2395,28 @@
       <c r="F16" s="1">
         <v>1</v>
       </c>
-      <c r="L16" s="30"/>
-      <c r="M16" s="30"/>
-      <c r="N16" s="30"/>
-      <c r="O16" s="30"/>
-      <c r="P16" s="30"/>
-      <c r="Q16" s="30"/>
-      <c r="R16" s="30"/>
-      <c r="S16" s="30"/>
-      <c r="T16" s="30"/>
-      <c r="U16" s="30"/>
-      <c r="V16" s="30"/>
+      <c r="H16" s="35">
+        <v>14</v>
+      </c>
+      <c r="I16" s="35" t="s">
+        <v>321</v>
+      </c>
+      <c r="J16" s="36">
+        <v>44206</v>
+      </c>
+      <c r="L16" s="27">
+        <v>14</v>
+      </c>
+      <c r="M16" s="27"/>
+      <c r="N16" s="27"/>
+      <c r="O16" s="27"/>
+      <c r="P16" s="27"/>
+      <c r="Q16" s="27"/>
+      <c r="R16" s="27"/>
+      <c r="S16" s="27"/>
+      <c r="T16" s="27"/>
+      <c r="U16" s="27"/>
+      <c r="V16" s="27"/>
     </row>
     <row r="17" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="B17" s="1">
@@ -2330,6 +2434,9 @@
       <c r="F17" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="L17" s="31">
+        <v>15</v>
+      </c>
     </row>
     <row r="18" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="B18" s="1">
@@ -2364,7 +2471,7 @@
       <c r="F19" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="O19" s="33"/>
+      <c r="O19" s="30"/>
     </row>
     <row r="20" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="B20" s="1">
@@ -2479,7 +2586,7 @@
         <v>74</v>
       </c>
       <c r="N26" s="6"/>
-      <c r="O26" s="32" t="s">
+      <c r="O26" s="29" t="s">
         <v>285</v>
       </c>
       <c r="P26" s="5" t="s">
@@ -2528,13 +2635,13 @@
       </c>
       <c r="M27" s="8"/>
       <c r="N27" s="8"/>
-      <c r="P27" s="29">
+      <c r="P27" s="26">
         <v>1</v>
       </c>
-      <c r="Q27" s="29" t="s">
+      <c r="Q27" s="26" t="s">
         <v>288</v>
       </c>
-      <c r="R27" s="29" t="s">
+      <c r="R27" s="26" t="s">
         <v>301</v>
       </c>
     </row>
@@ -2574,13 +2681,13 @@
       </c>
       <c r="M28" s="8"/>
       <c r="N28" s="8"/>
-      <c r="P28" s="29">
+      <c r="P28" s="26">
         <v>2</v>
       </c>
-      <c r="Q28" s="29" t="s">
+      <c r="Q28" s="26" t="s">
         <v>289</v>
       </c>
-      <c r="R28" s="29" t="s">
+      <c r="R28" s="26" t="s">
         <v>301</v>
       </c>
     </row>
@@ -2620,13 +2727,13 @@
       </c>
       <c r="M29" s="8"/>
       <c r="N29" s="8"/>
-      <c r="P29" s="29">
+      <c r="P29" s="26">
         <v>3</v>
       </c>
-      <c r="Q29" s="29" t="s">
+      <c r="Q29" s="26" t="s">
         <v>290</v>
       </c>
-      <c r="R29" s="29" t="s">
+      <c r="R29" s="26" t="s">
         <v>301</v>
       </c>
     </row>
@@ -2666,13 +2773,13 @@
       </c>
       <c r="M30" s="8"/>
       <c r="N30" s="8"/>
-      <c r="P30" s="29">
+      <c r="P30" s="26">
         <v>4</v>
       </c>
-      <c r="Q30" s="29" t="s">
+      <c r="Q30" s="26" t="s">
         <v>291</v>
       </c>
-      <c r="R30" s="29" t="s">
+      <c r="R30" s="26" t="s">
         <v>301</v>
       </c>
     </row>
@@ -2712,13 +2819,13 @@
       </c>
       <c r="M31" s="8"/>
       <c r="N31" s="8"/>
-      <c r="P31" s="29">
+      <c r="P31" s="26">
         <v>5</v>
       </c>
-      <c r="Q31" s="29" t="s">
+      <c r="Q31" s="26" t="s">
         <v>292</v>
       </c>
-      <c r="R31" s="29" t="s">
+      <c r="R31" s="26" t="s">
         <v>301</v>
       </c>
     </row>
@@ -2758,13 +2865,13 @@
       </c>
       <c r="M32" s="8"/>
       <c r="N32" s="8"/>
-      <c r="P32" s="29">
+      <c r="P32" s="26">
         <v>6</v>
       </c>
-      <c r="Q32" s="29" t="s">
+      <c r="Q32" s="26" t="s">
         <v>293</v>
       </c>
-      <c r="R32" s="29" t="s">
+      <c r="R32" s="26" t="s">
         <v>302</v>
       </c>
     </row>
@@ -2804,13 +2911,13 @@
       </c>
       <c r="M33" s="8"/>
       <c r="N33" s="8"/>
-      <c r="P33" s="29">
+      <c r="P33" s="26">
         <v>7</v>
       </c>
-      <c r="Q33" s="29" t="s">
+      <c r="Q33" s="26" t="s">
         <v>294</v>
       </c>
-      <c r="R33" s="29" t="s">
+      <c r="R33" s="26" t="s">
         <v>302</v>
       </c>
     </row>
@@ -2850,13 +2957,13 @@
       </c>
       <c r="M34" s="8"/>
       <c r="N34" s="8"/>
-      <c r="P34" s="29">
+      <c r="P34" s="26">
         <v>8</v>
       </c>
-      <c r="Q34" s="29" t="s">
+      <c r="Q34" s="26" t="s">
         <v>295</v>
       </c>
-      <c r="R34" s="29" t="s">
+      <c r="R34" s="26" t="s">
         <v>302</v>
       </c>
     </row>
@@ -2898,13 +3005,13 @@
         <v>118</v>
       </c>
       <c r="N35" s="8"/>
-      <c r="P35" s="29">
+      <c r="P35" s="26">
         <v>9</v>
       </c>
-      <c r="Q35" s="29" t="s">
+      <c r="Q35" s="26" t="s">
         <v>278</v>
       </c>
-      <c r="R35" s="29" t="s">
+      <c r="R35" s="26" t="s">
         <v>302</v>
       </c>
     </row>
@@ -2944,13 +3051,13 @@
       </c>
       <c r="M36" s="8"/>
       <c r="N36" s="8"/>
-      <c r="P36" s="29">
+      <c r="P36" s="26">
         <v>10</v>
       </c>
-      <c r="Q36" s="29" t="s">
+      <c r="Q36" s="26" t="s">
         <v>296</v>
       </c>
-      <c r="R36" s="29" t="s">
+      <c r="R36" s="26" t="s">
         <v>303</v>
       </c>
     </row>
@@ -2990,13 +3097,13 @@
       </c>
       <c r="M37" s="8"/>
       <c r="N37" s="8"/>
-      <c r="P37" s="29">
+      <c r="P37" s="26">
         <v>11</v>
       </c>
-      <c r="Q37" s="29" t="s">
+      <c r="Q37" s="26" t="s">
         <v>297</v>
       </c>
-      <c r="R37" s="29" t="s">
+      <c r="R37" s="26" t="s">
         <v>304</v>
       </c>
     </row>
@@ -3036,13 +3143,13 @@
       </c>
       <c r="M38" s="8"/>
       <c r="N38" s="8"/>
-      <c r="P38" s="29">
+      <c r="P38" s="26">
         <v>12</v>
       </c>
-      <c r="Q38" s="29" t="s">
+      <c r="Q38" s="26" t="s">
         <v>298</v>
       </c>
-      <c r="R38" s="29" t="s">
+      <c r="R38" s="26" t="s">
         <v>304</v>
       </c>
     </row>
@@ -3082,13 +3189,13 @@
       </c>
       <c r="M39" s="8"/>
       <c r="N39" s="8"/>
-      <c r="P39" s="29">
+      <c r="P39" s="26">
         <v>13</v>
       </c>
-      <c r="Q39" s="29" t="s">
+      <c r="Q39" s="26" t="s">
         <v>299</v>
       </c>
-      <c r="R39" s="29" t="s">
+      <c r="R39" s="26" t="s">
         <v>304</v>
       </c>
     </row>
@@ -3128,13 +3235,13 @@
       </c>
       <c r="M40" s="8"/>
       <c r="N40" s="8"/>
-      <c r="P40" s="29">
+      <c r="P40" s="26">
         <v>14</v>
       </c>
-      <c r="Q40" s="29" t="s">
+      <c r="Q40" s="26" t="s">
         <v>300</v>
       </c>
-      <c r="R40" s="29" t="s">
+      <c r="R40" s="26" t="s">
         <v>305</v>
       </c>
     </row>
@@ -3174,11 +3281,11 @@
       </c>
       <c r="M41" s="8"/>
       <c r="N41" s="8"/>
-      <c r="P41" s="29">
+      <c r="P41" s="26">
         <v>15</v>
       </c>
-      <c r="Q41" s="29"/>
-      <c r="R41" s="29" t="s">
+      <c r="Q41" s="26"/>
+      <c r="R41" s="26" t="s">
         <v>306</v>
       </c>
     </row>
@@ -3218,13 +3325,13 @@
       </c>
       <c r="M42" s="8"/>
       <c r="N42" s="8"/>
-      <c r="P42" s="29">
+      <c r="P42" s="26">
         <v>16</v>
       </c>
-      <c r="Q42" s="29" t="s">
+      <c r="Q42" s="26" t="s">
         <v>314</v>
       </c>
-      <c r="R42" s="29" t="s">
+      <c r="R42" s="26" t="s">
         <v>307</v>
       </c>
     </row>
@@ -3266,13 +3373,13 @@
         <v>166</v>
       </c>
       <c r="N43" s="8"/>
-      <c r="P43" s="29">
+      <c r="P43" s="26">
         <v>17</v>
       </c>
-      <c r="Q43" s="29" t="s">
+      <c r="Q43" s="26" t="s">
         <v>313</v>
       </c>
-      <c r="R43" s="29" t="s">
+      <c r="R43" s="26" t="s">
         <v>308</v>
       </c>
     </row>
@@ -3312,11 +3419,11 @@
       </c>
       <c r="M44" s="8"/>
       <c r="N44" s="8"/>
-      <c r="P44" s="29">
+      <c r="P44" s="26">
         <v>18</v>
       </c>
-      <c r="Q44" s="29"/>
-      <c r="R44" s="29" t="s">
+      <c r="Q44" s="26"/>
+      <c r="R44" s="26" t="s">
         <v>309</v>
       </c>
     </row>
@@ -3356,9 +3463,9 @@
       </c>
       <c r="M45" s="8"/>
       <c r="N45" s="8"/>
-      <c r="P45" s="29"/>
-      <c r="Q45" s="29"/>
-      <c r="R45" s="29"/>
+      <c r="P45" s="26"/>
+      <c r="Q45" s="26"/>
+      <c r="R45" s="26"/>
     </row>
     <row r="46" spans="2:18" ht="19" x14ac:dyDescent="0.2">
       <c r="B46" s="11">
@@ -3396,9 +3503,9 @@
       </c>
       <c r="M46" s="8"/>
       <c r="N46" s="8"/>
-      <c r="P46" s="29"/>
-      <c r="Q46" s="29"/>
-      <c r="R46" s="29"/>
+      <c r="P46" s="26"/>
+      <c r="Q46" s="26"/>
+      <c r="R46" s="26"/>
     </row>
     <row r="50" spans="2:6" ht="21" x14ac:dyDescent="0.25">
       <c r="B50" s="15" t="s">
@@ -3423,7 +3530,7 @@
       </c>
     </row>
     <row r="53" spans="2:6" ht="36" x14ac:dyDescent="0.25">
-      <c r="B53" s="22" t="s">
+      <c r="B53" s="32" t="s">
         <v>220</v>
       </c>
       <c r="C53" s="17" t="s">
@@ -3438,7 +3545,7 @@
       </c>
     </row>
     <row r="54" spans="2:6" ht="54" x14ac:dyDescent="0.25">
-      <c r="B54" s="23"/>
+      <c r="B54" s="33"/>
       <c r="C54" s="17" t="s">
         <v>230</v>
       </c>
@@ -3451,7 +3558,7 @@
       </c>
     </row>
     <row r="55" spans="2:6" ht="72" x14ac:dyDescent="0.25">
-      <c r="B55" s="23"/>
+      <c r="B55" s="33"/>
       <c r="C55" s="17" t="s">
         <v>231</v>
       </c>
@@ -3464,7 +3571,7 @@
       </c>
     </row>
     <row r="56" spans="2:6" ht="54" x14ac:dyDescent="0.25">
-      <c r="B56" s="23"/>
+      <c r="B56" s="33"/>
       <c r="C56" s="17" t="s">
         <v>226</v>
       </c>
@@ -3477,7 +3584,7 @@
       </c>
     </row>
     <row r="57" spans="2:6" ht="54" x14ac:dyDescent="0.25">
-      <c r="B57" s="23"/>
+      <c r="B57" s="33"/>
       <c r="C57" s="17" t="s">
         <v>232</v>
       </c>
@@ -3490,7 +3597,7 @@
       </c>
     </row>
     <row r="58" spans="2:6" ht="54" x14ac:dyDescent="0.25">
-      <c r="B58" s="23"/>
+      <c r="B58" s="33"/>
       <c r="C58" s="19" t="s">
         <v>235</v>
       </c>
@@ -3503,7 +3610,7 @@
       </c>
     </row>
     <row r="59" spans="2:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="B59" s="23"/>
+      <c r="B59" s="33"/>
       <c r="C59" s="17" t="s">
         <v>237</v>
       </c>
@@ -3518,7 +3625,7 @@
       </c>
     </row>
     <row r="60" spans="2:6" ht="72" x14ac:dyDescent="0.25">
-      <c r="B60" s="23"/>
+      <c r="B60" s="33"/>
       <c r="C60" s="17" t="s">
         <v>240</v>
       </c>
@@ -3531,14 +3638,14 @@
       </c>
     </row>
     <row r="61" spans="2:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="B61" s="24"/>
+      <c r="B61" s="34"/>
       <c r="C61" s="17"/>
       <c r="D61" s="20"/>
       <c r="E61" s="17"/>
       <c r="F61" s="17"/>
     </row>
     <row r="62" spans="2:6" ht="54" x14ac:dyDescent="0.25">
-      <c r="B62" s="22" t="s">
+      <c r="B62" s="32" t="s">
         <v>242</v>
       </c>
       <c r="C62" s="17" t="s">
@@ -3553,7 +3660,7 @@
       </c>
     </row>
     <row r="63" spans="2:6" ht="120" x14ac:dyDescent="0.25">
-      <c r="B63" s="23"/>
+      <c r="B63" s="33"/>
       <c r="C63" s="17" t="s">
         <v>246</v>
       </c>
@@ -3568,42 +3675,42 @@
       </c>
     </row>
     <row r="64" spans="2:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="B64" s="23"/>
+      <c r="B64" s="33"/>
       <c r="C64" s="17"/>
       <c r="D64" s="20"/>
       <c r="E64" s="17"/>
       <c r="F64" s="17"/>
     </row>
     <row r="65" spans="2:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="B65" s="23"/>
+      <c r="B65" s="33"/>
       <c r="C65" s="17"/>
       <c r="D65" s="20"/>
       <c r="E65" s="17"/>
       <c r="F65" s="17"/>
     </row>
     <row r="66" spans="2:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="B66" s="23"/>
+      <c r="B66" s="33"/>
       <c r="C66" s="17"/>
       <c r="D66" s="20"/>
       <c r="E66" s="17"/>
       <c r="F66" s="17"/>
     </row>
     <row r="67" spans="2:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="B67" s="23"/>
+      <c r="B67" s="33"/>
       <c r="C67" s="17"/>
       <c r="D67" s="20"/>
       <c r="E67" s="17"/>
       <c r="F67" s="17"/>
     </row>
     <row r="68" spans="2:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="B68" s="23"/>
+      <c r="B68" s="33"/>
       <c r="C68" s="17"/>
       <c r="D68" s="20"/>
       <c r="E68" s="17"/>
       <c r="F68" s="17"/>
     </row>
     <row r="69" spans="2:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="B69" s="24"/>
+      <c r="B69" s="34"/>
       <c r="C69" s="17"/>
       <c r="D69" s="20"/>
       <c r="E69" s="17"/>

</xml_diff>

<commit_message>
dernière sauvegarde de la bdd
</commit_message>
<xml_diff>
--- a/bdd/infos_bdd.xlsx
+++ b/bdd/infos_bdd.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marieeonnet/Documents/Documents - MacBook Pro de Marie/Cours_DUT_Caen/Projet2A/dut2021_pret_instruments_voyage/bdd/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC1A2DDC-2973-F348-82A5-CB603AEA53B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E19B472-CA28-844B-A897-91F528FA919A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32700" yWindow="1020" windowWidth="33040" windowHeight="17660" xr2:uid="{1C6F6E9A-B456-E643-B447-123029CC3B3E}"/>
+    <workbookView xWindow="52640" yWindow="0" windowWidth="14560" windowHeight="21600" xr2:uid="{1C6F6E9A-B456-E643-B447-123029CC3B3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="326">
   <si>
     <t>Vil_nom</t>
   </si>
@@ -1000,6 +1000,34 @@
   </si>
   <si>
     <t>Gliga</t>
+  </si>
+  <si>
+    <t>Violon électrique prêté avec son micro Yamaha SRT, préampli externe, écouteurs et deux câbles.
+Un boîtier de commande externe, dotée d’une connexion d’entrée auxiliaire peut être utilisé pour activer une réverbération d’une grande clarté. Le violon silencieux permet de jouer en casque idéal lorsque l’on souhaite jouer en toute discrétion.</t>
+  </si>
+  <si>
+    <t>Système allemand
+Corps en grenadille (Dalbergia melanoxylon)
+22 clés
+6 anneaux
+Baril normal
+Plateau plat surélevé pour le trou de pouce
+Levier de Fa à gauche
+Levier de Mib à gauche
+Double clé Fa/Do
+Clé latérale Mib/Sib avec patte en métal
+Couplage des clés La et Sol#
+Liège synthétique
+Repose-pouce réglable avec anneau pour sangle
+Etui souple avec sangles sac à dos, ligature en textile BG et bec M3D incl.</t>
+  </si>
+  <si>
+    <t>Sonorité, ergonomie et fiabilité sont les qualités essentielles de la Prodige.
+Pour la première fois sur ce segment, les opérations essentielles pour une acoustique parfaite, à savoir le moulage et l’usinage de la perce, sont entièrement réalisées en France et en Allemagne afin de garantir des dimensions constantes.
+La nouvelle perce de la Prodige, inspirée du célèbre modèle E13, permet une facilité de jeu et d’émission sans précédent. Les rapports de notes sont totalement justes et équilibrés. Le pavillon a lui aussi été entièrement retravaillé afin d’optimiser la projection globale de l’instrument. L'innovation: une perce texturée.</t>
+  </si>
+  <si>
+    <t>CLARINETTE CRAMPON</t>
   </si>
 </sst>
 </file>
@@ -1255,6 +1283,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1264,10 +1296,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1585,8 +1613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D70755CD-10D4-DA48-863B-E92693C8657B}">
   <dimension ref="A2:V81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F12" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="T31" sqref="T31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2010,7 +2038,7 @@
       </c>
       <c r="V8" s="27"/>
     </row>
-    <row r="9" spans="1:22" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" ht="409.6" x14ac:dyDescent="0.2">
       <c r="B9" s="1">
         <v>7</v>
       </c>
@@ -2053,7 +2081,9 @@
       <c r="Q9" s="27" t="s">
         <v>282</v>
       </c>
-      <c r="R9" s="27"/>
+      <c r="R9" s="27" t="s">
+        <v>323</v>
+      </c>
       <c r="S9" s="27" t="s">
         <v>283</v>
       </c>
@@ -2285,7 +2315,7 @@
       </c>
       <c r="V13" s="27"/>
     </row>
-    <row r="14" spans="1:22" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22" ht="356" x14ac:dyDescent="0.2">
       <c r="B14" s="1">
         <v>12</v>
       </c>
@@ -2328,7 +2358,9 @@
       <c r="Q14" s="27" t="s">
         <v>318</v>
       </c>
-      <c r="R14" s="27"/>
+      <c r="R14" s="27" t="s">
+        <v>322</v>
+      </c>
       <c r="S14" s="27" t="s">
         <v>319</v>
       </c>
@@ -2395,13 +2427,13 @@
       <c r="F16" s="1">
         <v>1</v>
       </c>
-      <c r="H16" s="35">
+      <c r="H16" s="32">
         <v>14</v>
       </c>
-      <c r="I16" s="35" t="s">
+      <c r="I16" s="32" t="s">
         <v>321</v>
       </c>
-      <c r="J16" s="36">
+      <c r="J16" s="33">
         <v>44206</v>
       </c>
       <c r="L16" s="27">
@@ -2418,7 +2450,7 @@
       <c r="U16" s="27"/>
       <c r="V16" s="27"/>
     </row>
-    <row r="17" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" ht="409.6" x14ac:dyDescent="0.2">
       <c r="B17" s="1">
         <v>15</v>
       </c>
@@ -2436,6 +2468,24 @@
       </c>
       <c r="L17" s="31">
         <v>15</v>
+      </c>
+      <c r="M17" s="31">
+        <v>8</v>
+      </c>
+      <c r="N17" s="31">
+        <v>6</v>
+      </c>
+      <c r="O17" s="31">
+        <v>14</v>
+      </c>
+      <c r="P17" s="31">
+        <v>10</v>
+      </c>
+      <c r="Q17" s="31" t="s">
+        <v>325</v>
+      </c>
+      <c r="R17" s="18" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="18" spans="1:18" ht="17" x14ac:dyDescent="0.2">
@@ -3530,7 +3580,7 @@
       </c>
     </row>
     <row r="53" spans="2:6" ht="36" x14ac:dyDescent="0.25">
-      <c r="B53" s="32" t="s">
+      <c r="B53" s="34" t="s">
         <v>220</v>
       </c>
       <c r="C53" s="17" t="s">
@@ -3545,7 +3595,7 @@
       </c>
     </row>
     <row r="54" spans="2:6" ht="54" x14ac:dyDescent="0.25">
-      <c r="B54" s="33"/>
+      <c r="B54" s="35"/>
       <c r="C54" s="17" t="s">
         <v>230</v>
       </c>
@@ -3558,7 +3608,7 @@
       </c>
     </row>
     <row r="55" spans="2:6" ht="72" x14ac:dyDescent="0.25">
-      <c r="B55" s="33"/>
+      <c r="B55" s="35"/>
       <c r="C55" s="17" t="s">
         <v>231</v>
       </c>
@@ -3571,7 +3621,7 @@
       </c>
     </row>
     <row r="56" spans="2:6" ht="54" x14ac:dyDescent="0.25">
-      <c r="B56" s="33"/>
+      <c r="B56" s="35"/>
       <c r="C56" s="17" t="s">
         <v>226</v>
       </c>
@@ -3584,7 +3634,7 @@
       </c>
     </row>
     <row r="57" spans="2:6" ht="54" x14ac:dyDescent="0.25">
-      <c r="B57" s="33"/>
+      <c r="B57" s="35"/>
       <c r="C57" s="17" t="s">
         <v>232</v>
       </c>
@@ -3597,7 +3647,7 @@
       </c>
     </row>
     <row r="58" spans="2:6" ht="54" x14ac:dyDescent="0.25">
-      <c r="B58" s="33"/>
+      <c r="B58" s="35"/>
       <c r="C58" s="19" t="s">
         <v>235</v>
       </c>
@@ -3610,7 +3660,7 @@
       </c>
     </row>
     <row r="59" spans="2:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="B59" s="33"/>
+      <c r="B59" s="35"/>
       <c r="C59" s="17" t="s">
         <v>237</v>
       </c>
@@ -3625,7 +3675,7 @@
       </c>
     </row>
     <row r="60" spans="2:6" ht="72" x14ac:dyDescent="0.25">
-      <c r="B60" s="33"/>
+      <c r="B60" s="35"/>
       <c r="C60" s="17" t="s">
         <v>240</v>
       </c>
@@ -3638,14 +3688,14 @@
       </c>
     </row>
     <row r="61" spans="2:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="B61" s="34"/>
+      <c r="B61" s="36"/>
       <c r="C61" s="17"/>
       <c r="D61" s="20"/>
       <c r="E61" s="17"/>
       <c r="F61" s="17"/>
     </row>
     <row r="62" spans="2:6" ht="54" x14ac:dyDescent="0.25">
-      <c r="B62" s="32" t="s">
+      <c r="B62" s="34" t="s">
         <v>242</v>
       </c>
       <c r="C62" s="17" t="s">
@@ -3660,7 +3710,7 @@
       </c>
     </row>
     <row r="63" spans="2:6" ht="120" x14ac:dyDescent="0.25">
-      <c r="B63" s="33"/>
+      <c r="B63" s="35"/>
       <c r="C63" s="17" t="s">
         <v>246</v>
       </c>
@@ -3675,42 +3725,42 @@
       </c>
     </row>
     <row r="64" spans="2:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="B64" s="33"/>
+      <c r="B64" s="35"/>
       <c r="C64" s="17"/>
       <c r="D64" s="20"/>
       <c r="E64" s="17"/>
       <c r="F64" s="17"/>
     </row>
     <row r="65" spans="2:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="B65" s="33"/>
+      <c r="B65" s="35"/>
       <c r="C65" s="17"/>
       <c r="D65" s="20"/>
       <c r="E65" s="17"/>
       <c r="F65" s="17"/>
     </row>
     <row r="66" spans="2:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="B66" s="33"/>
+      <c r="B66" s="35"/>
       <c r="C66" s="17"/>
       <c r="D66" s="20"/>
       <c r="E66" s="17"/>
       <c r="F66" s="17"/>
     </row>
     <row r="67" spans="2:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="B67" s="33"/>
+      <c r="B67" s="35"/>
       <c r="C67" s="17"/>
       <c r="D67" s="20"/>
       <c r="E67" s="17"/>
       <c r="F67" s="17"/>
     </row>
     <row r="68" spans="2:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="B68" s="33"/>
+      <c r="B68" s="35"/>
       <c r="C68" s="17"/>
       <c r="D68" s="20"/>
       <c r="E68" s="17"/>
       <c r="F68" s="17"/>
     </row>
     <row r="69" spans="2:6" ht="17" x14ac:dyDescent="0.25">
-      <c r="B69" s="34"/>
+      <c r="B69" s="36"/>
       <c r="C69" s="17"/>
       <c r="D69" s="20"/>
       <c r="E69" s="17"/>

</xml_diff>